<commit_message>
Staveni novi podobri rezultati.
</commit_message>
<xml_diff>
--- a/luDecomposition/rezultati.xlsx
+++ b/luDecomposition/rezultati.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,16 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
+    <sheet name="Лист6" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="rez_debug" localSheetId="0">Лист1!$A$1:$D$51</definedName>
     <definedName name="rez_debug" localSheetId="4">Лист5!$A$1:$D$51</definedName>
     <definedName name="rez_release" localSheetId="2">Лист3!$A$1:$D$51</definedName>
+    <definedName name="rez2_release" localSheetId="5">Лист6!$A$1:$D$134</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,11 +62,21 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" name="rez2_release" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="D:\projects\cuda\luDecomposition\rez2_release.csv" decimal="," thousands="." semicolon="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="12">
   <si>
     <t>N</t>
   </si>
@@ -96,6 +109,9 @@
   </si>
   <si>
     <t>vkupno vreme (ms)</t>
+  </si>
+  <si>
+    <t>cuda LU release build</t>
   </si>
 </sst>
 </file>
@@ -167,7 +183,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1643,19 +1658,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="400864624"/>
-        <c:axId val="400871696"/>
+        <c:axId val="-614181504"/>
+        <c:axId val="-614169536"/>
         <c:extLst/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="400864624"/>
+        <c:axId val="-614181504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1722,12 +1736,12 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400871696"/>
+        <c:crossAx val="-614169536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="400871696"/>
+        <c:axId val="-614169536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,7 +1762,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1809,7 +1822,7 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400864624"/>
+        <c:crossAx val="-614181504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1823,6 +1836,2554 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="mk-MK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="mk-MK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="mk-MK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="mk-MK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист6!$D$1:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>LU on CPU release build</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>prosecno vreme (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист6!$A$3:$A$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>864</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>928</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>992</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1056</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1088</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1184</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1216</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1248</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1312</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1344</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1376</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1408</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1472</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1504</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1568</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1664</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1696</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1728</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1760</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1824</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1856</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1888</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2080</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист6!$D$3:$D$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>9.5909500000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3973200000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.195604</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44767899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84870299999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.44553</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2455099999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.39194</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6877000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.44198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.4670900000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.975999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.918099999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.303099999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.370100000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25.9344</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.782299999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36.4407</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42.864899999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49.450899999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>58.428699999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>66.065399999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>75.370599999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>85.791999999999987</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>97.058599999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>109.46899999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>123.048</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>137.58100000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>153.22399999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>170.41300000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>189.804</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>218.797</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>231.333</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>254.46400000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>280.31299999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>307.70699999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>347.35399999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>378.04900000000004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>413.553</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>443.25299999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>477.77599999999995</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>521.61400000000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>560.99400000000003</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>600.95500000000004</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>653.22499999999991</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>706.00300000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>763.09</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>828.65</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>891.13800000000003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>943.93499999999995</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1001.65</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1076.8500000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1144.1099999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1209.8</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1299.92</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1371.92</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1445.21</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1544.02</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1652.1999999999998</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1705.54</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1810.74</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1904.42</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1993.35</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2134.66</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2207.4899999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист6!$F$1:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>cuda LU release build</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>prosecno vreme (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист6!$A$3:$A$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>864</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>928</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>992</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1056</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1088</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1184</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1216</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1248</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1312</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1344</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1376</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1408</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1472</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1504</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1568</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1664</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1696</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1728</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1760</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1824</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1856</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1888</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2080</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист6!$F$3:$F$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0.24185699999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41752600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72147099999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.10717</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.69676</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.57029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7386200000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1416700000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.95486</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1552100000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.755800000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.870200000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.487100000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.590900000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.418199999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.770200000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38.830199999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45.615699999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>53.243099999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61.669400000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>70.934200000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>80.880799999999994</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>92.024600000000007</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>104.026</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>117.307</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>131.27600000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>146.31</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>162.52500000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>180.06899999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>199.274</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>218.852</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>240.399</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>262.83999999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>287.01600000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>312.77499999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>339.37400000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>367.89800000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>397.524</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>428.97800000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>462.52499999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>496.88099999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>533.976</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>572.02700000000004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>611.50099999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>654.24400000000003</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>697.43200000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>743.774</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>790.89099999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>841.15</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>893.40300000000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>946.57100000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1001.84</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1060.31</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1120.51</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1183.97</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1247.24</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1315.17</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1384.22</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1456.66</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1532.27</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1607.73</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1687</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1771.85</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1851.77</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1944.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-614171712"/>
+        <c:axId val="-614180416"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$B$1:$B$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="1">
+                        <c:v>povtoruvanja</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$A$3:$A$67</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="65"/>
+                      <c:pt idx="0">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>96</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>160</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>192</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>224</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>544</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>576</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>608</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>640</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>672</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>704</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>736</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>768</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>800</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>832</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>864</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>896</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>928</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>960</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>992</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>1056</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>1088</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>1120</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>1152</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>1184</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>1216</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>1248</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>1280</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>1312</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>1344</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>1376</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>1408</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>1440</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>1472</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>1504</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>1536</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>1568</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>1600</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>1632</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1664</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>1696</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>1728</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>1760</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>1792</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>1824</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>1856</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>1888</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>1920</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>1952</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>1984</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>2080</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$B$3:$B$67</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="65"/>
+                      <c:pt idx="0">
+                        <c:v>100000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>12587</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3800</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1661</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>899</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>562</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>391</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>295</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>237</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>175</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>157</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>145</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>136</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>129</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>124</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>117</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>114</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>112</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>109</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>108</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>107</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>106</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>105</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>105</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>104</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>104</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>103</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>103</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>103</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>102</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>102</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>102</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>102</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>102</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>101</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>100</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$C$1:$C$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>LU on CPU release build</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>vkupno vreme (ms)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$A$3:$A$67</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="65"/>
+                      <c:pt idx="0">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>96</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>160</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>192</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>224</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>544</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>576</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>608</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>640</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>672</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>704</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>736</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>768</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>800</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>832</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>864</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>896</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>928</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>960</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>992</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>1056</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>1088</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>1120</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>1152</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>1184</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>1216</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>1248</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>1280</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>1312</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>1344</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>1376</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>1408</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>1440</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>1472</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>1504</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>1536</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>1568</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>1600</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>1632</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1664</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>1696</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>1728</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>1760</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>1792</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>1824</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>1856</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>1888</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>1920</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>1952</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>1984</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>2080</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$C$3:$C$67</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="65"/>
+                      <c:pt idx="0">
+                        <c:v>959.09500000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>805.23</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>743.29399999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>743.596</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>762.98400000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>812.38800000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>877.99599999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1000.6200000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1110.98</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1288.4000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1481.74</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1723.24</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2018.13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>2353.2199999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>2756.7400000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>3215.87</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>3693.88</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4263.5600000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>4886.5999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>5538.5</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>6427.16</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>7201.13</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>8140.03</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>9179.75</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>10288.199999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>11494.300000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>12920.1</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>14308.400000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>15935.3</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>17552.600000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>19549.800000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>22536.100000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>23595.9</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>25955.300000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>28591.899999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>31386.1</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>35430.100000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>38183</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>41768.799999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>44768.6</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>48255.299999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>52683</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>56660.4</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>60696.399999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>65975.7</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>71306.299999999988</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>77072.100000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>83693.700000000012</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>89113.8</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>94393.5</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>100165</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>107685</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>114411</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>120980</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>129991.99999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>137192</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>144521</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>154402</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>165220</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>170554</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>181074</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>190442</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>199335</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>213466</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>220749</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$E$1:$E$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>cuda LU release build</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>vkupno vreme (ms)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$A$3:$A$67</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="65"/>
+                      <c:pt idx="0">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>96</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>160</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>192</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>224</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>544</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>576</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>608</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>640</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>672</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>704</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>736</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>768</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>800</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>832</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>864</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>896</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>928</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>960</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>992</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>1056</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>1088</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>1120</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>1152</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>1184</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>1216</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>1248</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>1280</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>1312</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>1344</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>1376</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>1408</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>1440</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>1472</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>1504</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>1536</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>1568</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>1600</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>1632</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1664</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>1696</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>1728</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>1760</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>1792</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>1824</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>1856</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>1888</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>1920</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>1952</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>1984</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>2080</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист6!$E$3:$E$67</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="65"/>
+                      <c:pt idx="0">
+                        <c:v>24185.7</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>5255.4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2741.59</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1839.01</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1525.39</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1444.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1461.8</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1516.79</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1648.3</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1831.04</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>2057.2600000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2334.61</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2680.63</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>3072.36</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>3536.94</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>4063.5</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>4659.63</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>5337.04</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>6069.72</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>6906.98</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>7802.76</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>8816.01</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>9938.66</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>11130.8</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>12434.5</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>13784</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>15362.6</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>16902.599999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>18727.2</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>20525.2</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>22541.8</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>24761.1</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>26809.7</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>29275.599999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>31903.1</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>34616.1</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>37525.599999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>40149.9</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>43326.8</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>46715</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>50185</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>53931.5</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>57774.7</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>61761.599999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>66078.600000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>70440.7</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>75121.2</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>79880</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>84115</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>89340.3</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>94657.1</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>100184</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>106031</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>112051</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>118397</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>124724</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>131517</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>138422</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>145666</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>153227</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>160773</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>168700</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>177185</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>185177</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>194405</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-614171712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="mk-MK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-614180416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-614180416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="mk-MK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-614171712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1891,6 +4452,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2446,6 +5047,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2481,6 +5598,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Графикон 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rez_debug" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -2491,6 +5643,10 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rez_debug" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rez2_release" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5660,7 +8816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F30" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
@@ -7774,4 +10930,1362 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>100000</v>
+      </c>
+      <c r="C3">
+        <v>959.09500000000003</v>
+      </c>
+      <c r="D3">
+        <v>9.5909500000000009E-3</v>
+      </c>
+      <c r="E3">
+        <v>24185.7</v>
+      </c>
+      <c r="F3">
+        <v>0.24185699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>12587</v>
+      </c>
+      <c r="C4">
+        <v>805.23</v>
+      </c>
+      <c r="D4">
+        <v>6.3973200000000008E-2</v>
+      </c>
+      <c r="E4">
+        <v>5255.4</v>
+      </c>
+      <c r="F4">
+        <v>0.41752600000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>3800</v>
+      </c>
+      <c r="C5">
+        <v>743.29399999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.195604</v>
+      </c>
+      <c r="E5">
+        <v>2741.59</v>
+      </c>
+      <c r="F5">
+        <v>0.72147099999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>128</v>
+      </c>
+      <c r="B6">
+        <v>1661</v>
+      </c>
+      <c r="C6">
+        <v>743.596</v>
+      </c>
+      <c r="D6">
+        <v>0.44767899999999999</v>
+      </c>
+      <c r="E6">
+        <v>1839.01</v>
+      </c>
+      <c r="F6">
+        <v>1.10717</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>160</v>
+      </c>
+      <c r="B7">
+        <v>899</v>
+      </c>
+      <c r="C7">
+        <v>762.98400000000004</v>
+      </c>
+      <c r="D7">
+        <v>0.84870299999999999</v>
+      </c>
+      <c r="E7">
+        <v>1525.39</v>
+      </c>
+      <c r="F7">
+        <v>1.69676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>192</v>
+      </c>
+      <c r="B8">
+        <v>562</v>
+      </c>
+      <c r="C8">
+        <v>812.38800000000003</v>
+      </c>
+      <c r="D8">
+        <v>1.44553</v>
+      </c>
+      <c r="E8">
+        <v>1444.5</v>
+      </c>
+      <c r="F8">
+        <v>2.57029</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>224</v>
+      </c>
+      <c r="B9">
+        <v>391</v>
+      </c>
+      <c r="C9">
+        <v>877.99599999999998</v>
+      </c>
+      <c r="D9">
+        <v>2.2455099999999999</v>
+      </c>
+      <c r="E9">
+        <v>1461.8</v>
+      </c>
+      <c r="F9">
+        <v>3.7386200000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>256</v>
+      </c>
+      <c r="B10">
+        <v>295</v>
+      </c>
+      <c r="C10">
+        <v>1000.6200000000001</v>
+      </c>
+      <c r="D10">
+        <v>3.39194</v>
+      </c>
+      <c r="E10">
+        <v>1516.79</v>
+      </c>
+      <c r="F10">
+        <v>5.1416700000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>288</v>
+      </c>
+      <c r="B11">
+        <v>237</v>
+      </c>
+      <c r="C11">
+        <v>1110.98</v>
+      </c>
+      <c r="D11">
+        <v>4.6877000000000004</v>
+      </c>
+      <c r="E11">
+        <v>1648.3</v>
+      </c>
+      <c r="F11">
+        <v>6.95486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>320</v>
+      </c>
+      <c r="B12">
+        <v>200</v>
+      </c>
+      <c r="C12">
+        <v>1288.4000000000001</v>
+      </c>
+      <c r="D12">
+        <v>6.44198</v>
+      </c>
+      <c r="E12">
+        <v>1831.04</v>
+      </c>
+      <c r="F12">
+        <v>9.1552100000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>352</v>
+      </c>
+      <c r="B13">
+        <v>175</v>
+      </c>
+      <c r="C13">
+        <v>1481.74</v>
+      </c>
+      <c r="D13">
+        <v>8.4670900000000007</v>
+      </c>
+      <c r="E13">
+        <v>2057.2600000000002</v>
+      </c>
+      <c r="F13">
+        <v>11.755800000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>384</v>
+      </c>
+      <c r="B14">
+        <v>157</v>
+      </c>
+      <c r="C14">
+        <v>1723.24</v>
+      </c>
+      <c r="D14">
+        <v>10.975999999999999</v>
+      </c>
+      <c r="E14">
+        <v>2334.61</v>
+      </c>
+      <c r="F14">
+        <v>14.870200000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>416</v>
+      </c>
+      <c r="B15">
+        <v>145</v>
+      </c>
+      <c r="C15">
+        <v>2018.13</v>
+      </c>
+      <c r="D15">
+        <v>13.918099999999999</v>
+      </c>
+      <c r="E15">
+        <v>2680.63</v>
+      </c>
+      <c r="F15">
+        <v>18.487100000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>448</v>
+      </c>
+      <c r="B16">
+        <v>136</v>
+      </c>
+      <c r="C16">
+        <v>2353.2199999999998</v>
+      </c>
+      <c r="D16">
+        <v>17.303099999999997</v>
+      </c>
+      <c r="E16">
+        <v>3072.36</v>
+      </c>
+      <c r="F16">
+        <v>22.590900000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>480</v>
+      </c>
+      <c r="B17">
+        <v>129</v>
+      </c>
+      <c r="C17">
+        <v>2756.7400000000002</v>
+      </c>
+      <c r="D17">
+        <v>21.370100000000001</v>
+      </c>
+      <c r="E17">
+        <v>3536.94</v>
+      </c>
+      <c r="F17">
+        <v>27.418199999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>512</v>
+      </c>
+      <c r="B18">
+        <v>124</v>
+      </c>
+      <c r="C18">
+        <v>3215.87</v>
+      </c>
+      <c r="D18">
+        <v>25.9344</v>
+      </c>
+      <c r="E18">
+        <v>4063.5</v>
+      </c>
+      <c r="F18">
+        <v>32.770200000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>544</v>
+      </c>
+      <c r="B19">
+        <v>120</v>
+      </c>
+      <c r="C19">
+        <v>3693.88</v>
+      </c>
+      <c r="D19">
+        <v>30.782299999999999</v>
+      </c>
+      <c r="E19">
+        <v>4659.63</v>
+      </c>
+      <c r="F19">
+        <v>38.830199999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>576</v>
+      </c>
+      <c r="B20">
+        <v>117</v>
+      </c>
+      <c r="C20">
+        <v>4263.5600000000004</v>
+      </c>
+      <c r="D20">
+        <v>36.4407</v>
+      </c>
+      <c r="E20">
+        <v>5337.04</v>
+      </c>
+      <c r="F20">
+        <v>45.615699999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>608</v>
+      </c>
+      <c r="B21">
+        <v>114</v>
+      </c>
+      <c r="C21">
+        <v>4886.5999999999995</v>
+      </c>
+      <c r="D21">
+        <v>42.864899999999999</v>
+      </c>
+      <c r="E21">
+        <v>6069.72</v>
+      </c>
+      <c r="F21">
+        <v>53.243099999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>640</v>
+      </c>
+      <c r="B22">
+        <v>112</v>
+      </c>
+      <c r="C22">
+        <v>5538.5</v>
+      </c>
+      <c r="D22">
+        <v>49.450899999999997</v>
+      </c>
+      <c r="E22">
+        <v>6906.98</v>
+      </c>
+      <c r="F22">
+        <v>61.669400000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>672</v>
+      </c>
+      <c r="B23">
+        <v>110</v>
+      </c>
+      <c r="C23">
+        <v>6427.16</v>
+      </c>
+      <c r="D23">
+        <v>58.428699999999999</v>
+      </c>
+      <c r="E23">
+        <v>7802.76</v>
+      </c>
+      <c r="F23">
+        <v>70.934200000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>704</v>
+      </c>
+      <c r="B24">
+        <v>109</v>
+      </c>
+      <c r="C24">
+        <v>7201.13</v>
+      </c>
+      <c r="D24">
+        <v>66.065399999999997</v>
+      </c>
+      <c r="E24">
+        <v>8816.01</v>
+      </c>
+      <c r="F24">
+        <v>80.880799999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>736</v>
+      </c>
+      <c r="B25">
+        <v>108</v>
+      </c>
+      <c r="C25">
+        <v>8140.03</v>
+      </c>
+      <c r="D25">
+        <v>75.370599999999996</v>
+      </c>
+      <c r="E25">
+        <v>9938.66</v>
+      </c>
+      <c r="F25">
+        <v>92.024600000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>768</v>
+      </c>
+      <c r="B26">
+        <v>107</v>
+      </c>
+      <c r="C26">
+        <v>9179.75</v>
+      </c>
+      <c r="D26">
+        <v>85.791999999999987</v>
+      </c>
+      <c r="E26">
+        <v>11130.8</v>
+      </c>
+      <c r="F26">
+        <v>104.026</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>800</v>
+      </c>
+      <c r="B27">
+        <v>106</v>
+      </c>
+      <c r="C27">
+        <v>10288.199999999999</v>
+      </c>
+      <c r="D27">
+        <v>97.058599999999998</v>
+      </c>
+      <c r="E27">
+        <v>12434.5</v>
+      </c>
+      <c r="F27">
+        <v>117.307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>832</v>
+      </c>
+      <c r="B28">
+        <v>105</v>
+      </c>
+      <c r="C28">
+        <v>11494.300000000001</v>
+      </c>
+      <c r="D28">
+        <v>109.46899999999999</v>
+      </c>
+      <c r="E28">
+        <v>13784</v>
+      </c>
+      <c r="F28">
+        <v>131.27600000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>864</v>
+      </c>
+      <c r="B29">
+        <v>105</v>
+      </c>
+      <c r="C29">
+        <v>12920.1</v>
+      </c>
+      <c r="D29">
+        <v>123.048</v>
+      </c>
+      <c r="E29">
+        <v>15362.6</v>
+      </c>
+      <c r="F29">
+        <v>146.31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>896</v>
+      </c>
+      <c r="B30">
+        <v>104</v>
+      </c>
+      <c r="C30">
+        <v>14308.400000000001</v>
+      </c>
+      <c r="D30">
+        <v>137.58100000000002</v>
+      </c>
+      <c r="E30">
+        <v>16902.599999999999</v>
+      </c>
+      <c r="F30">
+        <v>162.52500000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>928</v>
+      </c>
+      <c r="B31">
+        <v>104</v>
+      </c>
+      <c r="C31">
+        <v>15935.3</v>
+      </c>
+      <c r="D31">
+        <v>153.22399999999999</v>
+      </c>
+      <c r="E31">
+        <v>18727.2</v>
+      </c>
+      <c r="F31">
+        <v>180.06899999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>960</v>
+      </c>
+      <c r="B32">
+        <v>103</v>
+      </c>
+      <c r="C32">
+        <v>17552.600000000002</v>
+      </c>
+      <c r="D32">
+        <v>170.41300000000001</v>
+      </c>
+      <c r="E32">
+        <v>20525.2</v>
+      </c>
+      <c r="F32">
+        <v>199.274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>992</v>
+      </c>
+      <c r="B33">
+        <v>103</v>
+      </c>
+      <c r="C33">
+        <v>19549.800000000003</v>
+      </c>
+      <c r="D33">
+        <v>189.804</v>
+      </c>
+      <c r="E33">
+        <v>22541.8</v>
+      </c>
+      <c r="F33">
+        <v>218.852</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>1024</v>
+      </c>
+      <c r="B34">
+        <v>103</v>
+      </c>
+      <c r="C34">
+        <v>22536.100000000002</v>
+      </c>
+      <c r="D34">
+        <v>218.797</v>
+      </c>
+      <c r="E34">
+        <v>24761.1</v>
+      </c>
+      <c r="F34">
+        <v>240.399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>1056</v>
+      </c>
+      <c r="B35">
+        <v>102</v>
+      </c>
+      <c r="C35">
+        <v>23595.9</v>
+      </c>
+      <c r="D35">
+        <v>231.333</v>
+      </c>
+      <c r="E35">
+        <v>26809.7</v>
+      </c>
+      <c r="F35">
+        <v>262.83999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>1088</v>
+      </c>
+      <c r="B36">
+        <v>102</v>
+      </c>
+      <c r="C36">
+        <v>25955.300000000003</v>
+      </c>
+      <c r="D36">
+        <v>254.46400000000003</v>
+      </c>
+      <c r="E36">
+        <v>29275.599999999999</v>
+      </c>
+      <c r="F36">
+        <v>287.01600000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>1120</v>
+      </c>
+      <c r="B37">
+        <v>102</v>
+      </c>
+      <c r="C37">
+        <v>28591.899999999998</v>
+      </c>
+      <c r="D37">
+        <v>280.31299999999999</v>
+      </c>
+      <c r="E37">
+        <v>31903.1</v>
+      </c>
+      <c r="F37">
+        <v>312.77499999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>1152</v>
+      </c>
+      <c r="B38">
+        <v>102</v>
+      </c>
+      <c r="C38">
+        <v>31386.1</v>
+      </c>
+      <c r="D38">
+        <v>307.70699999999999</v>
+      </c>
+      <c r="E38">
+        <v>34616.1</v>
+      </c>
+      <c r="F38">
+        <v>339.37400000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>1184</v>
+      </c>
+      <c r="B39">
+        <v>102</v>
+      </c>
+      <c r="C39">
+        <v>35430.100000000006</v>
+      </c>
+      <c r="D39">
+        <v>347.35399999999998</v>
+      </c>
+      <c r="E39">
+        <v>37525.599999999999</v>
+      </c>
+      <c r="F39">
+        <v>367.89800000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>1216</v>
+      </c>
+      <c r="B40">
+        <v>101</v>
+      </c>
+      <c r="C40">
+        <v>38183</v>
+      </c>
+      <c r="D40">
+        <v>378.04900000000004</v>
+      </c>
+      <c r="E40">
+        <v>40149.9</v>
+      </c>
+      <c r="F40">
+        <v>397.524</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>1248</v>
+      </c>
+      <c r="B41">
+        <v>101</v>
+      </c>
+      <c r="C41">
+        <v>41768.799999999996</v>
+      </c>
+      <c r="D41">
+        <v>413.553</v>
+      </c>
+      <c r="E41">
+        <v>43326.8</v>
+      </c>
+      <c r="F41">
+        <v>428.97800000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>1280</v>
+      </c>
+      <c r="B42">
+        <v>101</v>
+      </c>
+      <c r="C42">
+        <v>44768.6</v>
+      </c>
+      <c r="D42">
+        <v>443.25299999999999</v>
+      </c>
+      <c r="E42">
+        <v>46715</v>
+      </c>
+      <c r="F42">
+        <v>462.52499999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>1312</v>
+      </c>
+      <c r="B43">
+        <v>101</v>
+      </c>
+      <c r="C43">
+        <v>48255.299999999996</v>
+      </c>
+      <c r="D43">
+        <v>477.77599999999995</v>
+      </c>
+      <c r="E43">
+        <v>50185</v>
+      </c>
+      <c r="F43">
+        <v>496.88099999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>1344</v>
+      </c>
+      <c r="B44">
+        <v>101</v>
+      </c>
+      <c r="C44">
+        <v>52683</v>
+      </c>
+      <c r="D44">
+        <v>521.61400000000003</v>
+      </c>
+      <c r="E44">
+        <v>53931.5</v>
+      </c>
+      <c r="F44">
+        <v>533.976</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>1376</v>
+      </c>
+      <c r="B45">
+        <v>101</v>
+      </c>
+      <c r="C45">
+        <v>56660.4</v>
+      </c>
+      <c r="D45">
+        <v>560.99400000000003</v>
+      </c>
+      <c r="E45">
+        <v>57774.7</v>
+      </c>
+      <c r="F45">
+        <v>572.02700000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>1408</v>
+      </c>
+      <c r="B46">
+        <v>101</v>
+      </c>
+      <c r="C46">
+        <v>60696.399999999994</v>
+      </c>
+      <c r="D46">
+        <v>600.95500000000004</v>
+      </c>
+      <c r="E46">
+        <v>61761.599999999999</v>
+      </c>
+      <c r="F46">
+        <v>611.50099999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>1440</v>
+      </c>
+      <c r="B47">
+        <v>101</v>
+      </c>
+      <c r="C47">
+        <v>65975.7</v>
+      </c>
+      <c r="D47">
+        <v>653.22499999999991</v>
+      </c>
+      <c r="E47">
+        <v>66078.600000000006</v>
+      </c>
+      <c r="F47">
+        <v>654.24400000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>1472</v>
+      </c>
+      <c r="B48">
+        <v>101</v>
+      </c>
+      <c r="C48">
+        <v>71306.299999999988</v>
+      </c>
+      <c r="D48">
+        <v>706.00300000000004</v>
+      </c>
+      <c r="E48">
+        <v>70440.7</v>
+      </c>
+      <c r="F48">
+        <v>697.43200000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>1504</v>
+      </c>
+      <c r="B49">
+        <v>101</v>
+      </c>
+      <c r="C49">
+        <v>77072.100000000006</v>
+      </c>
+      <c r="D49">
+        <v>763.09</v>
+      </c>
+      <c r="E49">
+        <v>75121.2</v>
+      </c>
+      <c r="F49">
+        <v>743.774</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>1536</v>
+      </c>
+      <c r="B50">
+        <v>101</v>
+      </c>
+      <c r="C50">
+        <v>83693.700000000012</v>
+      </c>
+      <c r="D50">
+        <v>828.65</v>
+      </c>
+      <c r="E50">
+        <v>79880</v>
+      </c>
+      <c r="F50">
+        <v>790.89099999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>1568</v>
+      </c>
+      <c r="B51">
+        <v>100</v>
+      </c>
+      <c r="C51">
+        <v>89113.8</v>
+      </c>
+      <c r="D51">
+        <v>891.13800000000003</v>
+      </c>
+      <c r="E51">
+        <v>84115</v>
+      </c>
+      <c r="F51">
+        <v>841.15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>1600</v>
+      </c>
+      <c r="B52">
+        <v>100</v>
+      </c>
+      <c r="C52">
+        <v>94393.5</v>
+      </c>
+      <c r="D52">
+        <v>943.93499999999995</v>
+      </c>
+      <c r="E52">
+        <v>89340.3</v>
+      </c>
+      <c r="F52">
+        <v>893.40300000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>1632</v>
+      </c>
+      <c r="B53">
+        <v>100</v>
+      </c>
+      <c r="C53">
+        <v>100165</v>
+      </c>
+      <c r="D53">
+        <v>1001.65</v>
+      </c>
+      <c r="E53">
+        <v>94657.1</v>
+      </c>
+      <c r="F53">
+        <v>946.57100000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>1664</v>
+      </c>
+      <c r="B54">
+        <v>100</v>
+      </c>
+      <c r="C54">
+        <v>107685</v>
+      </c>
+      <c r="D54">
+        <v>1076.8500000000001</v>
+      </c>
+      <c r="E54">
+        <v>100184</v>
+      </c>
+      <c r="F54">
+        <v>1001.84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>1696</v>
+      </c>
+      <c r="B55">
+        <v>100</v>
+      </c>
+      <c r="C55">
+        <v>114411</v>
+      </c>
+      <c r="D55">
+        <v>1144.1099999999999</v>
+      </c>
+      <c r="E55">
+        <v>106031</v>
+      </c>
+      <c r="F55">
+        <v>1060.31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>1728</v>
+      </c>
+      <c r="B56">
+        <v>100</v>
+      </c>
+      <c r="C56">
+        <v>120980</v>
+      </c>
+      <c r="D56">
+        <v>1209.8</v>
+      </c>
+      <c r="E56">
+        <v>112051</v>
+      </c>
+      <c r="F56">
+        <v>1120.51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>1760</v>
+      </c>
+      <c r="B57">
+        <v>100</v>
+      </c>
+      <c r="C57">
+        <v>129991.99999999999</v>
+      </c>
+      <c r="D57">
+        <v>1299.92</v>
+      </c>
+      <c r="E57">
+        <v>118397</v>
+      </c>
+      <c r="F57">
+        <v>1183.97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>1792</v>
+      </c>
+      <c r="B58">
+        <v>100</v>
+      </c>
+      <c r="C58">
+        <v>137192</v>
+      </c>
+      <c r="D58">
+        <v>1371.92</v>
+      </c>
+      <c r="E58">
+        <v>124724</v>
+      </c>
+      <c r="F58">
+        <v>1247.24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>1824</v>
+      </c>
+      <c r="B59">
+        <v>100</v>
+      </c>
+      <c r="C59">
+        <v>144521</v>
+      </c>
+      <c r="D59">
+        <v>1445.21</v>
+      </c>
+      <c r="E59">
+        <v>131517</v>
+      </c>
+      <c r="F59">
+        <v>1315.17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>1856</v>
+      </c>
+      <c r="B60">
+        <v>100</v>
+      </c>
+      <c r="C60">
+        <v>154402</v>
+      </c>
+      <c r="D60">
+        <v>1544.02</v>
+      </c>
+      <c r="E60">
+        <v>138422</v>
+      </c>
+      <c r="F60">
+        <v>1384.22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>1888</v>
+      </c>
+      <c r="B61">
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>165220</v>
+      </c>
+      <c r="D61">
+        <v>1652.1999999999998</v>
+      </c>
+      <c r="E61">
+        <v>145666</v>
+      </c>
+      <c r="F61">
+        <v>1456.66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>1920</v>
+      </c>
+      <c r="B62">
+        <v>100</v>
+      </c>
+      <c r="C62">
+        <v>170554</v>
+      </c>
+      <c r="D62">
+        <v>1705.54</v>
+      </c>
+      <c r="E62">
+        <v>153227</v>
+      </c>
+      <c r="F62">
+        <v>1532.27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>1952</v>
+      </c>
+      <c r="B63">
+        <v>100</v>
+      </c>
+      <c r="C63">
+        <v>181074</v>
+      </c>
+      <c r="D63">
+        <v>1810.74</v>
+      </c>
+      <c r="E63">
+        <v>160773</v>
+      </c>
+      <c r="F63">
+        <v>1607.73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>1984</v>
+      </c>
+      <c r="B64">
+        <v>100</v>
+      </c>
+      <c r="C64">
+        <v>190442</v>
+      </c>
+      <c r="D64">
+        <v>1904.42</v>
+      </c>
+      <c r="E64">
+        <v>168700</v>
+      </c>
+      <c r="F64">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>2016</v>
+      </c>
+      <c r="B65">
+        <v>100</v>
+      </c>
+      <c r="C65">
+        <v>199335</v>
+      </c>
+      <c r="D65">
+        <v>1993.35</v>
+      </c>
+      <c r="E65">
+        <v>177185</v>
+      </c>
+      <c r="F65">
+        <v>1771.85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <v>2048</v>
+      </c>
+      <c r="B66">
+        <v>100</v>
+      </c>
+      <c r="C66">
+        <v>213466</v>
+      </c>
+      <c r="D66">
+        <v>2134.66</v>
+      </c>
+      <c r="E66">
+        <v>185177</v>
+      </c>
+      <c r="F66">
+        <v>1851.77</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>2080</v>
+      </c>
+      <c r="B67">
+        <v>100</v>
+      </c>
+      <c r="C67">
+        <v>220749</v>
+      </c>
+      <c r="D67">
+        <v>2207.4899999999998</v>
+      </c>
+      <c r="E67">
+        <v>194405</v>
+      </c>
+      <c r="F67">
+        <v>1944.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ispraveni presmetkite za bandwidth vo LU.
</commit_message>
<xml_diff>
--- a/luDecomposition/rezultati.xlsx
+++ b/luDecomposition/rezultati.xlsx
@@ -102,9 +102,6 @@
     <t>memoriski pristapi</t>
   </si>
   <si>
-    <t>bandwidth(words/s)</t>
-  </si>
-  <si>
     <t>CPU release</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>GPU release</t>
+  </si>
+  <si>
+    <t>bandwidth(GB/s)</t>
   </si>
 </sst>
 </file>
@@ -1668,12 +1668,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-831967792"/>
-        <c:axId val="-831973232"/>
+        <c:axId val="271781936"/>
+        <c:axId val="271782480"/>
         <c:extLst/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-831967792"/>
+        <c:axId val="271781936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,12 +1777,12 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-831973232"/>
+        <c:crossAx val="271782480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-831973232"/>
+        <c:axId val="271782480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1898,7 +1898,7 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-831967792"/>
+        <c:crossAx val="271781936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2022,7 +2022,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>bandwidth</a:t>
+              <a:t>bandwidth GB/s</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="mk-MK" baseline="0"/>
@@ -2080,7 +2080,7 @@
                   <c:v>CPU debug</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bandwidth(words/s)</c:v>
+                  <c:v>bandwidth(GB/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2272,151 +2272,151 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>799643.54125229106</c:v>
+                  <c:v>3.1985741650091644</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>851752.42920337257</c:v>
+                  <c:v>3.4070097168134903</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>857790.86332985072</c:v>
+                  <c:v>3.4311634533194026</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>869774.01360655332</c:v>
+                  <c:v>3.4790960544262131</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>876369.59163188748</c:v>
+                  <c:v>3.5054783665275502</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>881495.3685728549</c:v>
+                  <c:v>3.5259814742914197</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>878181.02967598033</c:v>
+                  <c:v>3.5127241187039218</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>878699.53851910366</c:v>
+                  <c:v>3.5147981540764146</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>880619.15605573566</c:v>
+                  <c:v>3.5224766242229428</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>890911.15422234952</c:v>
+                  <c:v>3.5636446168893983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>886721.14245513023</c:v>
+                  <c:v>3.5468845698205209</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>887690.67611573439</c:v>
+                  <c:v>3.550762704462938</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>890090.74722805666</c:v>
+                  <c:v>3.5603629889122268</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>883665.50236285175</c:v>
+                  <c:v>3.5346620094514076</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>887038.61975318496</c:v>
+                  <c:v>3.5481544790127399</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>890573.67579214531</c:v>
+                  <c:v>3.5622947031685817</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>891683.39320894657</c:v>
+                  <c:v>3.5667335728357865</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>892489.43765212898</c:v>
+                  <c:v>3.5699577506085158</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>892452.33883064415</c:v>
+                  <c:v>3.5698093553225765</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>894520.88811481406</c:v>
+                  <c:v>3.578083552459256</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>887552.8637123137</c:v>
+                  <c:v>3.5502114548492547</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>884498.35564981541</c:v>
+                  <c:v>3.537993422599262</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>889696.21329297742</c:v>
+                  <c:v>3.5587848531719097</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>892473.27971262555</c:v>
+                  <c:v>3.5698931188505019</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>889679.28351420537</c:v>
+                  <c:v>3.5587171340568218</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>890572.96633557067</c:v>
+                  <c:v>3.5622918653422824</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>885444.29484606977</c:v>
+                  <c:v>3.5417771793842787</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>889261.529162889</c:v>
+                  <c:v>3.5570461166515566</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>887928.79727889947</c:v>
+                  <c:v>3.5517151891155976</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>887393.82753367594</c:v>
+                  <c:v>3.5495753101347036</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>853557.31862685212</c:v>
+                  <c:v>3.4142292745074085</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>880240.69186146406</c:v>
+                  <c:v>3.5209627674458561</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>881906.03079683054</c:v>
+                  <c:v>3.527624123187322</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>886218.49801502808</c:v>
+                  <c:v>3.5448739920601127</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>874673.29563109821</c:v>
+                  <c:v>3.4986931825243928</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>884628.67936298903</c:v>
+                  <c:v>3.5385147174519558</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>884334.12550663273</c:v>
+                  <c:v>3.5373365020265308</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>887093.0919156943</c:v>
+                  <c:v>3.5483723676627767</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>882046.72825215315</c:v>
+                  <c:v>3.5281869130086125</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>886417.70447802765</c:v>
+                  <c:v>3.5456708179121108</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>883278.27737294685</c:v>
+                  <c:v>3.5331131094917874</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>868412.15827183961</c:v>
+                  <c:v>3.4736486330873584</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>876471.67855307227</c:v>
+                  <c:v>3.5058867142122891</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>877683.97057299758</c:v>
+                  <c:v>3.510735882291991</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>867250.18344871979</c:v>
+                  <c:v>3.4690007337948794</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>881382.58064338088</c:v>
+                  <c:v>3.5255303225735237</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>882494.40986065462</c:v>
+                  <c:v>3.5299776394426186</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>881135.97517295659</c:v>
+                  <c:v>3.524543900691826</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>880252.59797270317</c:v>
+                  <c:v>3.5210103918908127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2435,7 +2435,7 @@
                   <c:v>CPU release</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bandwidth(words/s)</c:v>
+                  <c:v>bandwidth(GB/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2627,151 +2627,151 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>3937877.9841448837</c:v>
+                  <c:v>15.751511936579535</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4570470.2071400071</c:v>
+                  <c:v>18.281880828560027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4676840.2247365555</c:v>
+                  <c:v>18.707360898946224</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4993833.6733019156</c:v>
+                  <c:v>19.97533469320766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5024308.6305633327</c:v>
+                  <c:v>20.097234522253331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5111729.3039612314</c:v>
+                  <c:v>20.446917215844923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5142895.4982902035</c:v>
+                  <c:v>20.571581993160812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5123972.0713731572</c:v>
+                  <c:v>20.495888285492629</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5185531.0727520837</c:v>
+                  <c:v>20.742124291008334</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5174882.6843699487</c:v>
+                  <c:v>20.699530737479794</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5234730.4703164073</c:v>
+                  <c:v>20.938921881265632</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5156504.8332593469</c:v>
+                  <c:v>20.626019333037387</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5212605.2430570573</c:v>
+                  <c:v>20.850420972228225</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5238155.4451023946</c:v>
+                  <c:v>20.952621780409579</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5257559.4744940232</c:v>
+                  <c:v>21.030237897976093</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5200607.3588612406</c:v>
+                  <c:v>20.802429435444964</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5265765.1245551603</c:v>
+                  <c:v>21.063060498220644</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5223737.231208425</c:v>
+                  <c:v>20.894948924833702</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5298385.3079945119</c:v>
+                  <c:v>21.193541231978045</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5289977.6100036809</c:v>
+                  <c:v>21.159910440014723</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5305168.8370090583</c:v>
+                  <c:v>21.220675348036231</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5320315.2307287613</c:v>
+                  <c:v>21.281260922915045</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5299993.8750104401</c:v>
+                  <c:v>21.199975500041759</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5245744.3429428134</c:v>
+                  <c:v>20.982977371771256</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5287360.1107576676</c:v>
+                  <c:v>21.14944044303067</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5296514.7937137038</c:v>
+                  <c:v>21.186059174854815</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5270171.0838462487</c:v>
+                  <c:v>21.080684335384991</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5283155.0220580688</c:v>
+                  <c:v>21.132620088232276</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5205321.131923412</c:v>
+                  <c:v>20.821284527693649</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5222329.4279807033</c:v>
+                  <c:v>20.889317711922814</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5135397.0410659714</c:v>
+                  <c:v>20.541588164263889</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4960938.1818852546</c:v>
+                  <c:v>19.843752727541016</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5103707.6411960134</c:v>
+                  <c:v>20.414830564784054</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5111319.1462390469</c:v>
+                  <c:v>20.44527658495619</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5035245.7990032807</c:v>
+                  <c:v>20.140983196013124</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5011102.1834518369</c:v>
+                  <c:v>20.044408733807348</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4919011.2753147231</c:v>
+                  <c:v>19.676045101258897</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4907512.2360615712</c:v>
+                  <c:v>19.630048944246283</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4847036.3288718928</c:v>
+                  <c:v>19.38814531548757</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4776307.076587229</c:v>
+                  <c:v>19.10522830634892</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4082791.3898139875</c:v>
+                  <c:v>16.33116555925595</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4673662.930419689</c:v>
+                  <c:v>18.694651721678756</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4661254.8201294895</c:v>
+                  <c:v>18.64501928051796</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4579849.0682273209</c:v>
+                  <c:v>18.319396272909287</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4356429.4580781274</c:v>
+                  <c:v>17.425717832312507</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4509187.7068344308</c:v>
+                  <c:v>18.036750827337723</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4465201.6342452234</c:v>
+                  <c:v>17.860806536980895</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4405695.9234593837</c:v>
+                  <c:v>17.622783693837533</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4387301.1442100154</c:v>
+                  <c:v>17.549204576840062</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,7 +2790,7 @@
                   <c:v>GPU debug</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bandwidth(words/s)</c:v>
+                  <c:v>bandwidth(GB/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2982,151 +2982,151 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>142960.97070236312</c:v>
+                  <c:v>0.57184388280945242</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>472404.78458030079</c:v>
+                  <c:v>1.8896191383212033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>807185.56452261575</c:v>
+                  <c:v>3.2287422580904628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1092524.3903690102</c:v>
+                  <c:v>4.3700975614760411</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1300849.7304011518</c:v>
+                  <c:v>5.2033989216046068</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1439521.7439438009</c:v>
+                  <c:v>5.7580869757752033</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1543809.6638403772</c:v>
+                  <c:v>6.1752386553615093</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1631932.3610883222</c:v>
+                  <c:v>6.5277294443532892</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1694022.1984337147</c:v>
+                  <c:v>6.7760887937348588</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1746089.2405130323</c:v>
+                  <c:v>6.9843569620521295</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1788906.3538739504</c:v>
+                  <c:v>7.155625415495801</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1824710.6232508037</c:v>
+                  <c:v>7.2988424930032147</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1847892.3207794433</c:v>
+                  <c:v>7.3915692831177733</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1873283.4022288548</c:v>
+                  <c:v>7.4931336089154197</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1890318.3416683406</c:v>
+                  <c:v>7.5612733666733618</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1908640.6840066973</c:v>
+                  <c:v>7.6345627360267887</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1923137.5573527575</c:v>
+                  <c:v>7.6925502294110295</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1936065.6479178108</c:v>
+                  <c:v>7.7442625916712435</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1944945.5317020158</c:v>
+                  <c:v>7.7797821268080636</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1953794.830263539</c:v>
+                  <c:v>7.8151793210541554</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1961093.6386538919</c:v>
+                  <c:v>7.844374554615567</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1968600.147403836</c:v>
+                  <c:v>7.8744005896153437</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1974668.5502593233</c:v>
+                  <c:v>7.8986742010372932</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1979559.8599990411</c:v>
+                  <c:v>7.9182394399961646</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1983821.1592645701</c:v>
+                  <c:v>7.9352846370582801</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1988669.7852581104</c:v>
+                  <c:v>7.9546791410324422</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1993547.3342399599</c:v>
+                  <c:v>7.9741893369598404</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1996722.8573960827</c:v>
+                  <c:v>7.9868914295843307</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2000797.2200224337</c:v>
+                  <c:v>8.0031888800897342</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2001659.8859392849</c:v>
+                  <c:v>8.0066395437571387</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2006427.7588495077</c:v>
+                  <c:v>8.0257110353980305</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2007907.7418668496</c:v>
+                  <c:v>8.0316309674673985</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2010760.7805709415</c:v>
+                  <c:v>8.0430431222837662</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2012768.0922489422</c:v>
+                  <c:v>8.0510723689957704</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2014246.7666846514</c:v>
+                  <c:v>8.056987066738607</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2016522.1781122237</c:v>
+                  <c:v>8.0660887124488951</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2018280.8280456585</c:v>
+                  <c:v>8.0731233121826342</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2020345.9014867074</c:v>
+                  <c:v>8.0813836059468294</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2021934.1974077767</c:v>
+                  <c:v>8.0877367896311068</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2021878.8082976369</c:v>
+                  <c:v>8.0875152331905493</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2024820.5253075038</c:v>
+                  <c:v>8.0992821012300151</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2024504.1475498562</c:v>
+                  <c:v>8.0980165901994265</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2026432.3101777059</c:v>
+                  <c:v>8.1057292407108239</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2028206.5302568567</c:v>
+                  <c:v>8.1128261210274264</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2028404.0077876442</c:v>
+                  <c:v>8.1136160311505758</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2029922.5972110995</c:v>
+                  <c:v>8.1196903888443988</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2030201.0155188444</c:v>
+                  <c:v>8.1208040620753756</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2030859.3061066866</c:v>
+                  <c:v>8.1234372244267465</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2032113.2075471699</c:v>
+                  <c:v>8.1284528301886798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3145,7 +3145,7 @@
                   <c:v>GPU release </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bandwidth(words/s)</c:v>
+                  <c:v>bandwidth(GB/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3337,151 +3337,151 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>160676.37665909805</c:v>
+                  <c:v>0.64270550663639214</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>655282.16042215587</c:v>
+                  <c:v>2.6211286416886233</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1291583.2465764396</c:v>
+                  <c:v>5.1663329863057577</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1922848.450378716</c:v>
+                  <c:v>7.6913938015148631</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2446783.40491811</c:v>
+                  <c:v>9.7871336196724403</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2783997.3840230764</c:v>
+                  <c:v>11.135989536092307</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3040423.4154764363</c:v>
+                  <c:v>12.161693661905744</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3289979.0439609829</c:v>
+                  <c:v>13.159916175843932</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3462487.1886407868</c:v>
+                  <c:v>13.849948754563149</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3605164.6677943012</c:v>
+                  <c:v>14.420658671177204</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3734558.4892165964</c:v>
+                  <c:v>14.938233956866386</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3832501.7170098443</c:v>
+                  <c:v>15.330006868039375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3914806.7691674917</c:v>
+                  <c:v>15.659227076669966</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3999291.5087321545</c:v>
+                  <c:v>15.99716603492862</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4051602.3582978225</c:v>
+                  <c:v>16.20640943319129</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4114775.1626921236</c:v>
+                  <c:v>16.459100650768491</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4161060.5767967924</c:v>
+                  <c:v>16.64424230718717</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4201168.2951408662</c:v>
+                  <c:v>16.804673180563466</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4232288.0947152479</c:v>
+                  <c:v>16.929152378860991</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4264736.0764451446</c:v>
+                  <c:v>17.058944305780578</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4290136.7943743048</c:v>
+                  <c:v>17.160547177497222</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4326179.9586552065</c:v>
+                  <c:v>17.304719834620826</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4343167.6953178896</c:v>
+                  <c:v>17.372670781271562</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4363819.1688686041</c:v>
+                  <c:v>17.455276675474419</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4373141.5767097492</c:v>
+                  <c:v>17.492566306839002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4395441.1012303568</c:v>
+                  <c:v>17.581764404921429</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4417649.2343016462</c:v>
+                  <c:v>17.670596937206586</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4434601.7260363298</c:v>
+                  <c:v>17.738406904145318</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4447572.8025944605</c:v>
+                  <c:v>17.790291210377841</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4448621.8783399314</c:v>
+                  <c:v>17.794487513359726</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4469584.4421699075</c:v>
+                  <c:v>17.878337768679629</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4474552.2740033688</c:v>
+                  <c:v>17.898209096013474</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4487042.1468178816</c:v>
+                  <c:v>17.948168587271521</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4495501.8535552025</c:v>
+                  <c:v>17.98200741422081</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4498859.8114709295</c:v>
+                  <c:v>17.995439245883716</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4510901.1799496925</c:v>
+                  <c:v>18.043604719798768</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4517864.4261234878</c:v>
+                  <c:v>18.071457704493948</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4530300.9161203988</c:v>
+                  <c:v>18.121203664481595</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4537589.4988066824</c:v>
+                  <c:v>18.150357995226731</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4539632.191956982</c:v>
+                  <c:v>18.158528767827928</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4551309.3773014648</c:v>
+                  <c:v>18.205237509205862</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4551506.4294686625</c:v>
+                  <c:v>18.206025717874653</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4561394.6537526883</c:v>
+                  <c:v>18.245578615010754</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4570241.961986511</c:v>
+                  <c:v>18.280967847946044</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4570053.5543980636</c:v>
+                  <c:v>18.280214217592256</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4578620.4901405629</c:v>
+                  <c:v>18.314481960562251</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4579349.0773002971</c:v>
+                  <c:v>18.317396309201186</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4586896.186095194</c:v>
+                  <c:v>18.347584744380775</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4589133.7088616928</c:v>
+                  <c:v>18.356534835446773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3496,11 +3496,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-874258832"/>
-        <c:axId val="-874260464"/>
+        <c:axId val="271787920"/>
+        <c:axId val="271789552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-874258832"/>
+        <c:axId val="271787920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3557,12 +3557,12 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-874260464"/>
+        <c:crossAx val="271789552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-874260464"/>
+        <c:axId val="271789552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3619,7 +3619,7 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-874258832"/>
+        <c:crossAx val="271787920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4777,12 +4777,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-831967248"/>
-        <c:axId val="-831971600"/>
+        <c:axId val="271792272"/>
+        <c:axId val="271792816"/>
         <c:extLst/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-831967248"/>
+        <c:axId val="271792272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4825,12 +4825,12 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-831971600"/>
+        <c:crossAx val="271792816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-831971600"/>
+        <c:axId val="271792816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4881,7 +4881,7 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-831967248"/>
+        <c:crossAx val="271792272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5005,7 +5005,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>bandwidth</a:t>
+              <a:t>bandwidth GB/s</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="mk-MK" baseline="0"/>
@@ -5063,7 +5063,7 @@
                   <c:v>CPU release</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bandwidth(words/s)</c:v>
+                  <c:v>bandwidth(GB/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5303,199 +5303,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="65"/>
                 <c:pt idx="0">
-                  <c:v>3630088.7816118319</c:v>
+                  <c:v>14.520355126447329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4225769.5409952914</c:v>
+                  <c:v>16.903078163981164</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4617328.8889797758</c:v>
+                  <c:v>18.469315555919103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4757694.6874881331</c:v>
+                  <c:v>19.030778749952535</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4886515.0706430869</c:v>
+                  <c:v>19.546060282572348</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4947400.6073896773</c:v>
+                  <c:v>19.789602429558709</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5049977.9560099933</c:v>
+                  <c:v>20.199911824039976</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4984842.8922681417</c:v>
+                  <c:v>19.939371569072566</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5131249.8666723548</c:v>
+                  <c:v>20.524999466689419</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5118426.3223418882</c:v>
+                  <c:v>20.473705289367555</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5180294.0561633334</c:v>
+                  <c:v>20.721176224653334</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5185679.3002915457</c:v>
+                  <c:v>20.74271720116618</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5197362.2836450385</c:v>
+                  <c:v>20.789449134580149</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5219688.9574700492</c:v>
+                  <c:v>20.878755829880195</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5196643.9090130599</c:v>
+                  <c:v>20.786575636052241</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5195493.8614350054</c:v>
+                  <c:v>20.78197544574002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5249154.7415235378</c:v>
+                  <c:v>20.996618966094154</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5262427.1213231357</c:v>
+                  <c:v>21.049708485292545</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5260598.7649568766</c:v>
+                  <c:v>21.042395059827506</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5317662.5703475568</c:v>
+                  <c:v>21.270650281390228</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5209214.2388928728</c:v>
+                  <c:v>20.836856955571491</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5296341.1407484105</c:v>
+                  <c:v>21.185364562993641</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5304079.4155811416</c:v>
+                  <c:v>21.21631766232457</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5293785.9007832902</c:v>
+                  <c:v>21.175143603133158</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5288351.5731733199</c:v>
+                  <c:v>21.153406292693283</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5273774.4566955036</c:v>
+                  <c:v>21.095097826782013</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5253767.1152720889</c:v>
+                  <c:v>21.015068461088354</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5240031.4578321129</c:v>
+                  <c:v>20.960125831328455</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5226995.2487860909</c:v>
+                  <c:v>20.907980995144364</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5202532.670629588</c:v>
+                  <c:v>20.810130682518352</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5153524.7729236474</c:v>
+                  <c:v>20.614099091694591</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4917064.5666988119</c:v>
+                  <c:v>19.668258266795249</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5100067.3833823968</c:v>
+                  <c:v>20.400269533529588</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5070583.5010060361</c:v>
+                  <c:v>20.282334004024143</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5020947.2981987996</c:v>
+                  <c:v>20.083789192795198</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4977065.897103413</c:v>
+                  <c:v>19.908263588413654</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4786474.9391111089</c:v>
+                  <c:v>19.145899756444436</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4763940.6743570277</c:v>
+                  <c:v>19.055762697428108</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4707691.6380729917</c:v>
+                  <c:v>18.830766552291966</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4738667.984198641</c:v>
+                  <c:v>18.954671936794565</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4734113.927865779</c:v>
+                  <c:v>18.936455711463111</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4661163.7264337223</c:v>
+                  <c:v>18.644654905734889</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4650802.197527959</c:v>
+                  <c:v>18.603208790111839</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4651386.9424499338</c:v>
+                  <c:v>18.605547769799735</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4577490.4512227802</c:v>
+                  <c:v>18.309961804891117</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4523832.9242227012</c:v>
+                  <c:v>18.095331696890803</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4464212.7350640157</c:v>
+                  <c:v>17.856850940256063</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4378926.2631991794</c:v>
+                  <c:v>17.515705052796719</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4331584.6479445379</c:v>
+                  <c:v>17.326338591778153</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4344705.938438558</c:v>
+                  <c:v>17.378823753754229</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4344865.7874507066</c:v>
+                  <c:v>17.379463149802827</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4283772.7965826243</c:v>
+                  <c:v>17.135091186330499</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4268955.2298293002</c:v>
+                  <c:v>17.075820919317199</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4269922.5657133413</c:v>
+                  <c:v>17.079690262853365</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4198697.7660163697</c:v>
+                  <c:v>16.794791064065482</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4199229.9959181296</c:v>
+                  <c:v>16.796919983672517</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4203581.6082091872</c:v>
+                  <c:v>16.814326432836751</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4145230.9477856504</c:v>
+                  <c:v>16.580923791142602</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4077586.3454787559</c:v>
+                  <c:v>16.310345381915024</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4154262.4623286468</c:v>
+                  <c:v>16.617049849314586</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4111763.1553950319</c:v>
+                  <c:v>16.447052621580127</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4104874.1433087238</c:v>
+                  <c:v>16.419496573234895</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4114515.0665964335</c:v>
+                  <c:v>16.458060266385733</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4027959.1129266489</c:v>
+                  <c:v>16.111836451706598</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4080455.5400024466</c:v>
+                  <c:v>16.321822160009784</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5514,7 +5514,7 @@
                   <c:v>GPU release</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>bandwidth(words/s)</c:v>
+                  <c:v>bandwidth(GB/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5754,199 +5754,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="65"/>
                 <c:pt idx="0">
-                  <c:v>143952.83163191474</c:v>
+                  <c:v>0.57581132652765898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>647471.05569473514</c:v>
+                  <c:v>2.5898842227789407</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1251842.416396501</c:v>
+                  <c:v>5.0073696655860038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1923751.5467362737</c:v>
+                  <c:v>7.6950061869450943</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2444187.7460571914</c:v>
+                  <c:v>9.7767509842287659</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2782415.9919697777</c:v>
+                  <c:v>11.129663967879113</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3033144.8502388583</c:v>
+                  <c:v>12.132579400955432</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3288481.7578724418</c:v>
+                  <c:v>13.153927031489768</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3458554.1621254776</c:v>
+                  <c:v>13.834216648501911</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3601533.9899357851</c:v>
+                  <c:v>14.406135959743139</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3731095.7995202364</c:v>
+                  <c:v>14.924383198080948</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3827656.3865987007</c:v>
+                  <c:v>15.310625546394801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3912858.587880197</c:v>
+                  <c:v>15.651434351520788</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3997928.3693876737</c:v>
+                  <c:v>15.991713477550695</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4050331.5316103902</c:v>
+                  <c:v>16.201326126441561</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4111723.9443152617</c:v>
+                  <c:v>16.446895777261048</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4161221.3174281875</c:v>
+                  <c:v>16.644885269712752</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4203958.9001155309</c:v>
+                  <c:v>16.815835600462123</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4235197.424642818</c:v>
+                  <c:v>16.940789698571269</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4264079.1056828834</c:v>
+                  <c:v>17.05631642273153</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4290844.4163746117</c:v>
+                  <c:v>17.163377665498448</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4326179.9586552065</c:v>
+                  <c:v>17.304719834620826</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4344182.4034008291</c:v>
+                  <c:v>17.376729613603317</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4365874.6851748601</c:v>
+                  <c:v>17.463498740699439</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4375527.4621292846</c:v>
+                  <c:v>17.502109848517136</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4397717.9073097901</c:v>
+                  <c:v>17.59087162923916</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4418464.4658601601</c:v>
+                  <c:v>17.673857863440638</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4435802.2950315336</c:v>
+                  <c:v>17.743209180126133</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4447745.6974826315</c:v>
+                  <c:v>17.790982789930531</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4449046.0371147264</c:v>
+                  <c:v>17.796184148458906</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4469502.7507173801</c:v>
+                  <c:v>17.878011002869517</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4475222.3428550037</c:v>
+                  <c:v>17.900889371420014</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4488715.1422918886</c:v>
+                  <c:v>17.954860569167558</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4495501.8535552025</c:v>
+                  <c:v>17.98200741422081</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4499837.9026456717</c:v>
+                  <c:v>17.999351610582686</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4512655.701379599</c:v>
+                  <c:v>18.050622805518394</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4519190.6887235045</c:v>
+                  <c:v>18.07676275489402</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4530551.634618287</c:v>
+                  <c:v>18.122206538473147</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4538414.5573898889</c:v>
+                  <c:v>18.153658229559554</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4541222.2042051787</c:v>
+                  <c:v>18.164888816820714</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4552087.9566737311</c:v>
+                  <c:v>18.208351826694923</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4553253.8091599625</c:v>
+                  <c:v>18.213015236639851</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4561099.6124308817</c:v>
+                  <c:v>18.244398449723526</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4571168.7143602381</c:v>
+                  <c:v>18.284674857440951</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4570360.9051057398</c:v>
+                  <c:v>18.281443620422959</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4579427.9815093083</c:v>
+                  <c:v>18.31771192603723</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4580149.4755127225</c:v>
+                  <c:v>18.320597902050892</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4587986.52153078</c:v>
+                  <c:v>18.351946086123121</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4589002.7700172383</c:v>
+                  <c:v>18.356011080068953</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4590447.9837206723</c:v>
+                  <c:v>18.361791934882689</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4597684.5012154393</c:v>
+                  <c:v>18.39073800486176</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4604508.440469536</c:v>
+                  <c:v>18.418033761878142</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4606345.6611745628</c:v>
+                  <c:v>18.425382644698249</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4610179.5789417317</c:v>
+                  <c:v>18.440718315766929</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4609889.7776126079</c:v>
+                  <c:v>18.439559110450435</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4619004.8555209907</c:v>
+                  <c:v>18.476019422083962</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4619218.9420379112</c:v>
+                  <c:v>18.476875768151643</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4623773.3077112017</c:v>
+                  <c:v>18.495093230844805</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4624955.8304614667</c:v>
+                  <c:v>18.499823321845867</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4624028.9244062733</c:v>
+                  <c:v>18.49611569762509</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4630960.4324109145</c:v>
+                  <c:v>18.523841729643657</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4633908.9602845283</c:v>
+                  <c:v>18.535635841138117</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4628872.9903772892</c:v>
+                  <c:v>18.515491961509159</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4643299.7618494742</c:v>
+                  <c:v>18.573199047397896</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4633401.8157969192</c:v>
+                  <c:v>18.533607263187676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5961,11 +5961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-749387216"/>
-        <c:axId val="-749384496"/>
+        <c:axId val="271779760"/>
+        <c:axId val="335065232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-749387216"/>
+        <c:axId val="271779760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6022,12 +6022,12 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-749384496"/>
+        <c:crossAx val="335065232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-749384496"/>
+        <c:axId val="335065232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6084,7 +6084,7 @@
             <a:endParaRPr lang="mk-MK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-749387216"/>
+        <c:crossAx val="271779760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8793,8 +8793,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView topLeftCell="K30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:T51"/>
+    <sheetView topLeftCell="K49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8812,6 +8812,7 @@
     <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -8855,16 +8856,16 @@
         <v>0</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -8909,16 +8910,16 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="R2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="S2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>16</v>
@@ -8968,20 +8969,20 @@
         <v>32</v>
       </c>
       <c r="P3">
-        <f>$T3/D3</f>
-        <v>799643.54125229106</v>
+        <f>$T3*4/(D3/1000)/10^9</f>
+        <v>3.1985741650091644</v>
       </c>
       <c r="Q3">
-        <f>$T3/G3</f>
-        <v>3937877.9841448837</v>
+        <f>$T3*4/(G3/1000)/10^9</f>
+        <v>15.751511936579535</v>
       </c>
       <c r="R3">
-        <f>$T3/J3</f>
-        <v>142960.97070236312</v>
+        <f>$T3*4/(J3/1000)/10^9</f>
+        <v>0.57184388280945242</v>
       </c>
       <c r="S3">
-        <f>$T3/M3</f>
-        <v>160676.37665909805</v>
+        <f>$T3*4/(M3/1000)/10^9</f>
+        <v>0.64270550663639214</v>
       </c>
       <c r="T3">
         <f>O3^3+2*O3^2</f>
@@ -9032,23 +9033,23 @@
         <v>64</v>
       </c>
       <c r="P4">
-        <f>$T4/D4</f>
-        <v>851752.42920337257</v>
+        <f t="shared" ref="P4:P51" si="0">$T4*4/(D4/1000)/10^9</f>
+        <v>3.4070097168134903</v>
       </c>
       <c r="Q4">
-        <f>$T4/G4</f>
-        <v>4570470.2071400071</v>
+        <f t="shared" ref="Q4:Q51" si="1">$T4*4/(G4/1000)/10^9</f>
+        <v>18.281880828560027</v>
       </c>
       <c r="R4">
-        <f>$T4/J4</f>
-        <v>472404.78458030079</v>
+        <f t="shared" ref="R4:R51" si="2">$T4*4/(J4/1000)/10^9</f>
+        <v>1.8896191383212033</v>
       </c>
       <c r="S4">
-        <f>$T4/M4</f>
-        <v>655282.16042215587</v>
+        <f t="shared" ref="S4:S51" si="3">$T4*4/(M4/1000)/10^9</f>
+        <v>2.6211286416886233</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T51" si="0">O4^3+2*O4^2</f>
+        <f t="shared" ref="T4:T51" si="4">O4^3+2*O4^2</f>
         <v>270336</v>
       </c>
     </row>
@@ -9096,23 +9097,23 @@
         <v>96</v>
       </c>
       <c r="P5">
-        <f>$T5/D5</f>
-        <v>857790.86332985072</v>
+        <f t="shared" si="0"/>
+        <v>3.4311634533194026</v>
       </c>
       <c r="Q5">
-        <f>$T5/G5</f>
-        <v>4676840.2247365555</v>
+        <f t="shared" si="1"/>
+        <v>18.707360898946224</v>
       </c>
       <c r="R5">
-        <f>$T5/J5</f>
-        <v>807185.56452261575</v>
+        <f t="shared" si="2"/>
+        <v>3.2287422580904628</v>
       </c>
       <c r="S5">
-        <f>$T5/M5</f>
-        <v>1291583.2465764396</v>
+        <f t="shared" si="3"/>
+        <v>5.1663329863057577</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>903168</v>
       </c>
     </row>
@@ -9160,23 +9161,23 @@
         <v>128</v>
       </c>
       <c r="P6">
-        <f>$T6/D6</f>
-        <v>869774.01360655332</v>
+        <f t="shared" si="0"/>
+        <v>3.4790960544262131</v>
       </c>
       <c r="Q6">
-        <f>$T6/G6</f>
-        <v>4993833.6733019156</v>
+        <f t="shared" si="1"/>
+        <v>19.97533469320766</v>
       </c>
       <c r="R6">
-        <f>$T6/J6</f>
-        <v>1092524.3903690102</v>
+        <f t="shared" si="2"/>
+        <v>4.3700975614760411</v>
       </c>
       <c r="S6">
-        <f>$T6/M6</f>
-        <v>1922848.450378716</v>
+        <f t="shared" si="3"/>
+        <v>7.6913938015148631</v>
       </c>
       <c r="T6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2129920</v>
       </c>
     </row>
@@ -9224,23 +9225,23 @@
         <v>160</v>
       </c>
       <c r="P7">
-        <f>$T7/D7</f>
-        <v>876369.59163188748</v>
+        <f t="shared" si="0"/>
+        <v>3.5054783665275502</v>
       </c>
       <c r="Q7">
-        <f>$T7/G7</f>
-        <v>5024308.6305633327</v>
+        <f t="shared" si="1"/>
+        <v>20.097234522253331</v>
       </c>
       <c r="R7">
-        <f>$T7/J7</f>
-        <v>1300849.7304011518</v>
+        <f t="shared" si="2"/>
+        <v>5.2033989216046068</v>
       </c>
       <c r="S7">
-        <f>$T7/M7</f>
-        <v>2446783.40491811</v>
+        <f t="shared" si="3"/>
+        <v>9.7871336196724403</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4147200</v>
       </c>
     </row>
@@ -9288,23 +9289,23 @@
         <v>192</v>
       </c>
       <c r="P8">
-        <f>$T8/D8</f>
-        <v>881495.3685728549</v>
+        <f t="shared" si="0"/>
+        <v>3.5259814742914197</v>
       </c>
       <c r="Q8">
-        <f>$T8/G8</f>
-        <v>5111729.3039612314</v>
+        <f t="shared" si="1"/>
+        <v>20.446917215844923</v>
       </c>
       <c r="R8">
-        <f>$T8/J8</f>
-        <v>1439521.7439438009</v>
+        <f t="shared" si="2"/>
+        <v>5.7580869757752033</v>
       </c>
       <c r="S8">
-        <f>$T8/M8</f>
-        <v>2783997.3840230764</v>
+        <f t="shared" si="3"/>
+        <v>11.135989536092307</v>
       </c>
       <c r="T8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7151616</v>
       </c>
     </row>
@@ -9352,23 +9353,23 @@
         <v>224</v>
       </c>
       <c r="P9">
-        <f>$T9/D9</f>
-        <v>878181.02967598033</v>
+        <f t="shared" si="0"/>
+        <v>3.5127241187039218</v>
       </c>
       <c r="Q9">
-        <f>$T9/G9</f>
-        <v>5142895.4982902035</v>
+        <f t="shared" si="1"/>
+        <v>20.571581993160812</v>
       </c>
       <c r="R9">
-        <f>$T9/J9</f>
-        <v>1543809.6638403772</v>
+        <f t="shared" si="2"/>
+        <v>6.1752386553615093</v>
       </c>
       <c r="S9">
-        <f>$T9/M9</f>
-        <v>3040423.4154764363</v>
+        <f t="shared" si="3"/>
+        <v>12.161693661905744</v>
       </c>
       <c r="T9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>11339776</v>
       </c>
     </row>
@@ -9416,23 +9417,23 @@
         <v>256</v>
       </c>
       <c r="P10">
-        <f>$T10/D10</f>
-        <v>878699.53851910366</v>
+        <f t="shared" si="0"/>
+        <v>3.5147981540764146</v>
       </c>
       <c r="Q10">
-        <f>$T10/G10</f>
-        <v>5123972.0713731572</v>
+        <f t="shared" si="1"/>
+        <v>20.495888285492629</v>
       </c>
       <c r="R10">
-        <f>$T10/J10</f>
-        <v>1631932.3610883222</v>
+        <f t="shared" si="2"/>
+        <v>6.5277294443532892</v>
       </c>
       <c r="S10">
-        <f>$T10/M10</f>
-        <v>3289979.0439609829</v>
+        <f t="shared" si="3"/>
+        <v>13.159916175843932</v>
       </c>
       <c r="T10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16908288</v>
       </c>
     </row>
@@ -9480,23 +9481,23 @@
         <v>288</v>
       </c>
       <c r="P11">
-        <f>$T11/D11</f>
-        <v>880619.15605573566</v>
+        <f t="shared" si="0"/>
+        <v>3.5224766242229428</v>
       </c>
       <c r="Q11">
-        <f>$T11/G11</f>
-        <v>5185531.0727520837</v>
+        <f t="shared" si="1"/>
+        <v>20.742124291008334</v>
       </c>
       <c r="R11">
-        <f>$T11/J11</f>
-        <v>1694022.1984337147</v>
+        <f t="shared" si="2"/>
+        <v>6.7760887937348588</v>
       </c>
       <c r="S11">
-        <f>$T11/M11</f>
-        <v>3462487.1886407868</v>
+        <f t="shared" si="3"/>
+        <v>13.849948754563149</v>
       </c>
       <c r="T11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>24053760</v>
       </c>
     </row>
@@ -9544,23 +9545,23 @@
         <v>320</v>
       </c>
       <c r="P12">
-        <f>$T12/D12</f>
-        <v>890911.15422234952</v>
+        <f t="shared" si="0"/>
+        <v>3.5636446168893983</v>
       </c>
       <c r="Q12">
-        <f>$T12/G12</f>
-        <v>5174882.6843699487</v>
+        <f t="shared" si="1"/>
+        <v>20.699530737479794</v>
       </c>
       <c r="R12">
-        <f>$T12/J12</f>
-        <v>1746089.2405130323</v>
+        <f t="shared" si="2"/>
+        <v>6.9843569620521295</v>
       </c>
       <c r="S12">
-        <f>$T12/M12</f>
-        <v>3605164.6677943012</v>
+        <f t="shared" si="3"/>
+        <v>14.420658671177204</v>
       </c>
       <c r="T12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>32972800</v>
       </c>
     </row>
@@ -9608,23 +9609,23 @@
         <v>352</v>
       </c>
       <c r="P13">
-        <f>$T13/D13</f>
-        <v>886721.14245513023</v>
+        <f t="shared" si="0"/>
+        <v>3.5468845698205209</v>
       </c>
       <c r="Q13">
-        <f>$T13/G13</f>
-        <v>5234730.4703164073</v>
+        <f t="shared" si="1"/>
+        <v>20.938921881265632</v>
       </c>
       <c r="R13">
-        <f>$T13/J13</f>
-        <v>1788906.3538739504</v>
+        <f t="shared" si="2"/>
+        <v>7.155625415495801</v>
       </c>
       <c r="S13">
-        <f>$T13/M13</f>
-        <v>3734558.4892165964</v>
+        <f t="shared" si="3"/>
+        <v>14.938233956866386</v>
       </c>
       <c r="T13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>43862016</v>
       </c>
     </row>
@@ -9672,23 +9673,23 @@
         <v>384</v>
       </c>
       <c r="P14">
-        <f>$T14/D14</f>
-        <v>887690.67611573439</v>
+        <f t="shared" si="0"/>
+        <v>3.550762704462938</v>
       </c>
       <c r="Q14">
-        <f>$T14/G14</f>
-        <v>5156504.8332593469</v>
+        <f t="shared" si="1"/>
+        <v>20.626019333037387</v>
       </c>
       <c r="R14">
-        <f>$T14/J14</f>
-        <v>1824710.6232508037</v>
+        <f t="shared" si="2"/>
+        <v>7.2988424930032147</v>
       </c>
       <c r="S14">
-        <f>$T14/M14</f>
-        <v>3832501.7170098443</v>
+        <f t="shared" si="3"/>
+        <v>15.330006868039375</v>
       </c>
       <c r="T14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>56918016</v>
       </c>
     </row>
@@ -9736,23 +9737,23 @@
         <v>416</v>
       </c>
       <c r="P15">
-        <f>$T15/D15</f>
-        <v>890090.74722805666</v>
+        <f t="shared" si="0"/>
+        <v>3.5603629889122268</v>
       </c>
       <c r="Q15">
-        <f>$T15/G15</f>
-        <v>5212605.2430570573</v>
+        <f t="shared" si="1"/>
+        <v>20.850420972228225</v>
       </c>
       <c r="R15">
-        <f>$T15/J15</f>
-        <v>1847892.3207794433</v>
+        <f t="shared" si="2"/>
+        <v>7.3915692831177733</v>
       </c>
       <c r="S15">
-        <f>$T15/M15</f>
-        <v>3914806.7691674917</v>
+        <f t="shared" si="3"/>
+        <v>15.659227076669966</v>
       </c>
       <c r="T15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>72337408</v>
       </c>
     </row>
@@ -9800,23 +9801,23 @@
         <v>448</v>
       </c>
       <c r="P16">
-        <f>$T16/D16</f>
-        <v>883665.50236285175</v>
+        <f t="shared" si="0"/>
+        <v>3.5346620094514076</v>
       </c>
       <c r="Q16">
-        <f>$T16/G16</f>
-        <v>5238155.4451023946</v>
+        <f t="shared" si="1"/>
+        <v>20.952621780409579</v>
       </c>
       <c r="R16">
-        <f>$T16/J16</f>
-        <v>1873283.4022288548</v>
+        <f t="shared" si="2"/>
+        <v>7.4931336089154197</v>
       </c>
       <c r="S16">
-        <f>$T16/M16</f>
-        <v>3999291.5087321545</v>
+        <f t="shared" si="3"/>
+        <v>15.99716603492862</v>
       </c>
       <c r="T16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>90316800</v>
       </c>
     </row>
@@ -9864,23 +9865,23 @@
         <v>480</v>
       </c>
       <c r="P17">
-        <f>$T17/D17</f>
-        <v>887038.61975318496</v>
+        <f t="shared" si="0"/>
+        <v>3.5481544790127399</v>
       </c>
       <c r="Q17">
-        <f>$T17/G17</f>
-        <v>5257559.4744940232</v>
+        <f t="shared" si="1"/>
+        <v>21.030237897976093</v>
       </c>
       <c r="R17">
-        <f>$T17/J17</f>
-        <v>1890318.3416683406</v>
+        <f t="shared" si="2"/>
+        <v>7.5612733666733618</v>
       </c>
       <c r="S17">
-        <f>$T17/M17</f>
-        <v>4051602.3582978225</v>
+        <f t="shared" si="3"/>
+        <v>16.20640943319129</v>
       </c>
       <c r="T17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>111052800</v>
       </c>
     </row>
@@ -9928,23 +9929,23 @@
         <v>512</v>
       </c>
       <c r="P18">
-        <f>$T18/D18</f>
-        <v>890573.67579214531</v>
+        <f t="shared" si="0"/>
+        <v>3.5622947031685817</v>
       </c>
       <c r="Q18">
-        <f>$T18/G18</f>
-        <v>5200607.3588612406</v>
+        <f t="shared" si="1"/>
+        <v>20.802429435444964</v>
       </c>
       <c r="R18">
-        <f>$T18/J18</f>
-        <v>1908640.6840066973</v>
+        <f t="shared" si="2"/>
+        <v>7.6345627360267887</v>
       </c>
       <c r="S18">
-        <f>$T18/M18</f>
-        <v>4114775.1626921236</v>
+        <f t="shared" si="3"/>
+        <v>16.459100650768491</v>
       </c>
       <c r="T18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>134742016</v>
       </c>
     </row>
@@ -9992,23 +9993,23 @@
         <v>544</v>
       </c>
       <c r="P19">
-        <f>$T19/D19</f>
-        <v>891683.39320894657</v>
+        <f t="shared" si="0"/>
+        <v>3.5667335728357865</v>
       </c>
       <c r="Q19">
-        <f>$T19/G19</f>
-        <v>5265765.1245551603</v>
+        <f t="shared" si="1"/>
+        <v>21.063060498220644</v>
       </c>
       <c r="R19">
-        <f>$T19/J19</f>
-        <v>1923137.5573527575</v>
+        <f t="shared" si="2"/>
+        <v>7.6925502294110295</v>
       </c>
       <c r="S19">
-        <f>$T19/M19</f>
-        <v>4161060.5767967924</v>
+        <f t="shared" si="3"/>
+        <v>16.64424230718717</v>
       </c>
       <c r="T19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>161581056</v>
       </c>
     </row>
@@ -10056,23 +10057,23 @@
         <v>576</v>
       </c>
       <c r="P20">
-        <f>$T20/D20</f>
-        <v>892489.43765212898</v>
+        <f t="shared" si="0"/>
+        <v>3.5699577506085158</v>
       </c>
       <c r="Q20">
-        <f>$T20/G20</f>
-        <v>5223737.231208425</v>
+        <f t="shared" si="1"/>
+        <v>20.894948924833702</v>
       </c>
       <c r="R20">
-        <f>$T20/J20</f>
-        <v>1936065.6479178108</v>
+        <f t="shared" si="2"/>
+        <v>7.7442625916712435</v>
       </c>
       <c r="S20">
-        <f>$T20/M20</f>
-        <v>4201168.2951408662</v>
+        <f t="shared" si="3"/>
+        <v>16.804673180563466</v>
       </c>
       <c r="T20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>191766528</v>
       </c>
     </row>
@@ -10120,23 +10121,23 @@
         <v>608</v>
       </c>
       <c r="P21">
-        <f>$T21/D21</f>
-        <v>892452.33883064415</v>
+        <f t="shared" si="0"/>
+        <v>3.5698093553225765</v>
       </c>
       <c r="Q21">
-        <f>$T21/G21</f>
-        <v>5298385.3079945119</v>
+        <f t="shared" si="1"/>
+        <v>21.193541231978045</v>
       </c>
       <c r="R21">
-        <f>$T21/J21</f>
-        <v>1944945.5317020158</v>
+        <f t="shared" si="2"/>
+        <v>7.7797821268080636</v>
       </c>
       <c r="S21">
-        <f>$T21/M21</f>
-        <v>4232288.0947152479</v>
+        <f t="shared" si="3"/>
+        <v>16.929152378860991</v>
       </c>
       <c r="T21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>225495040</v>
       </c>
     </row>
@@ -10184,23 +10185,23 @@
         <v>640</v>
       </c>
       <c r="P22">
-        <f>$T22/D22</f>
-        <v>894520.88811481406</v>
+        <f t="shared" si="0"/>
+        <v>3.578083552459256</v>
       </c>
       <c r="Q22">
-        <f>$T22/G22</f>
-        <v>5289977.6100036809</v>
+        <f t="shared" si="1"/>
+        <v>21.159910440014723</v>
       </c>
       <c r="R22">
-        <f>$T22/J22</f>
-        <v>1953794.830263539</v>
+        <f t="shared" si="2"/>
+        <v>7.8151793210541554</v>
       </c>
       <c r="S22">
-        <f>$T22/M22</f>
-        <v>4264736.0764451446</v>
+        <f t="shared" si="3"/>
+        <v>17.058944305780578</v>
       </c>
       <c r="T22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>262963200</v>
       </c>
     </row>
@@ -10248,23 +10249,23 @@
         <v>672</v>
       </c>
       <c r="P23">
-        <f>$T23/D23</f>
-        <v>887552.8637123137</v>
+        <f t="shared" si="0"/>
+        <v>3.5502114548492547</v>
       </c>
       <c r="Q23">
-        <f>$T23/G23</f>
-        <v>5305168.8370090583</v>
+        <f t="shared" si="1"/>
+        <v>21.220675348036231</v>
       </c>
       <c r="R23">
-        <f>$T23/J23</f>
-        <v>1961093.6386538919</v>
+        <f t="shared" si="2"/>
+        <v>7.844374554615567</v>
       </c>
       <c r="S23">
-        <f>$T23/M23</f>
-        <v>4290136.7943743048</v>
+        <f t="shared" si="3"/>
+        <v>17.160547177497222</v>
       </c>
       <c r="T23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>304367616</v>
       </c>
     </row>
@@ -10312,23 +10313,23 @@
         <v>704</v>
       </c>
       <c r="P24">
-        <f>$T24/D24</f>
-        <v>884498.35564981541</v>
+        <f t="shared" si="0"/>
+        <v>3.537993422599262</v>
       </c>
       <c r="Q24">
-        <f>$T24/G24</f>
-        <v>5320315.2307287613</v>
+        <f t="shared" si="1"/>
+        <v>21.281260922915045</v>
       </c>
       <c r="R24">
-        <f>$T24/J24</f>
-        <v>1968600.147403836</v>
+        <f t="shared" si="2"/>
+        <v>7.8744005896153437</v>
       </c>
       <c r="S24">
-        <f>$T24/M24</f>
-        <v>4326179.9586552065</v>
+        <f t="shared" si="3"/>
+        <v>17.304719834620826</v>
       </c>
       <c r="T24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>349904896</v>
       </c>
     </row>
@@ -10376,23 +10377,23 @@
         <v>736</v>
       </c>
       <c r="P25">
-        <f>$T25/D25</f>
-        <v>889696.21329297742</v>
+        <f t="shared" si="0"/>
+        <v>3.5587848531719097</v>
       </c>
       <c r="Q25">
-        <f>$T25/G25</f>
-        <v>5299993.8750104401</v>
+        <f t="shared" si="1"/>
+        <v>21.199975500041759</v>
       </c>
       <c r="R25">
-        <f>$T25/J25</f>
-        <v>1974668.5502593233</v>
+        <f t="shared" si="2"/>
+        <v>7.8986742010372932</v>
       </c>
       <c r="S25">
-        <f>$T25/M25</f>
-        <v>4343167.6953178896</v>
+        <f t="shared" si="3"/>
+        <v>17.372670781271562</v>
       </c>
       <c r="T25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>399771648</v>
       </c>
     </row>
@@ -10440,23 +10441,23 @@
         <v>768</v>
       </c>
       <c r="P26">
-        <f>$T26/D26</f>
-        <v>892473.27971262555</v>
+        <f t="shared" si="0"/>
+        <v>3.5698931188505019</v>
       </c>
       <c r="Q26">
-        <f>$T26/G26</f>
-        <v>5245744.3429428134</v>
+        <f t="shared" si="1"/>
+        <v>20.982977371771256</v>
       </c>
       <c r="R26">
-        <f>$T26/J26</f>
-        <v>1979559.8599990411</v>
+        <f t="shared" si="2"/>
+        <v>7.9182394399961646</v>
       </c>
       <c r="S26">
-        <f>$T26/M26</f>
-        <v>4363819.1688686041</v>
+        <f t="shared" si="3"/>
+        <v>17.455276675474419</v>
       </c>
       <c r="T26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>454164480</v>
       </c>
     </row>
@@ -10504,23 +10505,23 @@
         <v>800</v>
       </c>
       <c r="P27">
-        <f>$T27/D27</f>
-        <v>889679.28351420537</v>
+        <f t="shared" si="0"/>
+        <v>3.5587171340568218</v>
       </c>
       <c r="Q27">
-        <f>$T27/G27</f>
-        <v>5287360.1107576676</v>
+        <f t="shared" si="1"/>
+        <v>21.14944044303067</v>
       </c>
       <c r="R27">
-        <f>$T27/J27</f>
-        <v>1983821.1592645701</v>
+        <f t="shared" si="2"/>
+        <v>7.9352846370582801</v>
       </c>
       <c r="S27">
-        <f>$T27/M27</f>
-        <v>4373141.5767097492</v>
+        <f t="shared" si="3"/>
+        <v>17.492566306839002</v>
       </c>
       <c r="T27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>513280000</v>
       </c>
     </row>
@@ -10568,23 +10569,23 @@
         <v>832</v>
       </c>
       <c r="P28">
-        <f>$T28/D28</f>
-        <v>890572.96633557067</v>
+        <f t="shared" si="0"/>
+        <v>3.5622918653422824</v>
       </c>
       <c r="Q28">
-        <f>$T28/G28</f>
-        <v>5296514.7937137038</v>
+        <f t="shared" si="1"/>
+        <v>21.186059174854815</v>
       </c>
       <c r="R28">
-        <f>$T28/J28</f>
-        <v>1988669.7852581104</v>
+        <f t="shared" si="2"/>
+        <v>7.9546791410324422</v>
       </c>
       <c r="S28">
-        <f>$T28/M28</f>
-        <v>4395441.1012303568</v>
+        <f t="shared" si="3"/>
+        <v>17.581764404921429</v>
       </c>
       <c r="T28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>577314816</v>
       </c>
     </row>
@@ -10632,23 +10633,23 @@
         <v>864</v>
       </c>
       <c r="P29">
-        <f>$T29/D29</f>
-        <v>885444.29484606977</v>
+        <f t="shared" si="0"/>
+        <v>3.5417771793842787</v>
       </c>
       <c r="Q29">
-        <f>$T29/G29</f>
-        <v>5270171.0838462487</v>
+        <f t="shared" si="1"/>
+        <v>21.080684335384991</v>
       </c>
       <c r="R29">
-        <f>$T29/J29</f>
-        <v>1993547.3342399599</v>
+        <f t="shared" si="2"/>
+        <v>7.9741893369598404</v>
       </c>
       <c r="S29">
-        <f>$T29/M29</f>
-        <v>4417649.2343016462</v>
+        <f t="shared" si="3"/>
+        <v>17.670596937206586</v>
       </c>
       <c r="T29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>646465536</v>
       </c>
     </row>
@@ -10696,23 +10697,23 @@
         <v>896</v>
       </c>
       <c r="P30">
-        <f>$T30/D30</f>
-        <v>889261.529162889</v>
+        <f t="shared" si="0"/>
+        <v>3.5570461166515566</v>
       </c>
       <c r="Q30">
-        <f>$T30/G30</f>
-        <v>5283155.0220580688</v>
+        <f t="shared" si="1"/>
+        <v>21.132620088232276</v>
       </c>
       <c r="R30">
-        <f>$T30/J30</f>
-        <v>1996722.8573960827</v>
+        <f t="shared" si="2"/>
+        <v>7.9868914295843307</v>
       </c>
       <c r="S30">
-        <f>$T30/M30</f>
-        <v>4434601.7260363298</v>
+        <f t="shared" si="3"/>
+        <v>17.738406904145318</v>
       </c>
       <c r="T30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>720928768</v>
       </c>
     </row>
@@ -10760,23 +10761,23 @@
         <v>928</v>
       </c>
       <c r="P31">
-        <f>$T31/D31</f>
-        <v>887928.79727889947</v>
+        <f t="shared" si="0"/>
+        <v>3.5517151891155976</v>
       </c>
       <c r="Q31">
-        <f>$T31/G31</f>
-        <v>5205321.131923412</v>
+        <f t="shared" si="1"/>
+        <v>20.821284527693649</v>
       </c>
       <c r="R31">
-        <f>$T31/J31</f>
-        <v>2000797.2200224337</v>
+        <f t="shared" si="2"/>
+        <v>8.0031888800897342</v>
       </c>
       <c r="S31">
-        <f>$T31/M31</f>
-        <v>4447572.8025944605</v>
+        <f t="shared" si="3"/>
+        <v>17.790291210377841</v>
       </c>
       <c r="T31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>800901120</v>
       </c>
     </row>
@@ -10824,23 +10825,23 @@
         <v>960</v>
       </c>
       <c r="P32">
-        <f>$T32/D32</f>
-        <v>887393.82753367594</v>
+        <f t="shared" si="0"/>
+        <v>3.5495753101347036</v>
       </c>
       <c r="Q32">
-        <f>$T32/G32</f>
-        <v>5222329.4279807033</v>
+        <f t="shared" si="1"/>
+        <v>20.889317711922814</v>
       </c>
       <c r="R32">
-        <f>$T32/J32</f>
-        <v>2001659.8859392849</v>
+        <f t="shared" si="2"/>
+        <v>8.0066395437571387</v>
       </c>
       <c r="S32">
-        <f>$T32/M32</f>
-        <v>4448621.8783399314</v>
+        <f t="shared" si="3"/>
+        <v>17.794487513359726</v>
       </c>
       <c r="T32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>886579200</v>
       </c>
     </row>
@@ -10888,23 +10889,23 @@
         <v>992</v>
       </c>
       <c r="P33">
-        <f>$T33/D33</f>
-        <v>853557.31862685212</v>
+        <f t="shared" si="0"/>
+        <v>3.4142292745074085</v>
       </c>
       <c r="Q33">
-        <f>$T33/G33</f>
-        <v>5135397.0410659714</v>
+        <f t="shared" si="1"/>
+        <v>20.541588164263889</v>
       </c>
       <c r="R33">
-        <f>$T33/J33</f>
-        <v>2006427.7588495077</v>
+        <f t="shared" si="2"/>
+        <v>8.0257110353980305</v>
       </c>
       <c r="S33">
-        <f>$T33/M33</f>
-        <v>4469584.4421699075</v>
+        <f t="shared" si="3"/>
+        <v>17.878337768679629</v>
       </c>
       <c r="T33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>978159616</v>
       </c>
     </row>
@@ -10952,23 +10953,23 @@
         <v>1024</v>
       </c>
       <c r="P34">
-        <f>$T34/D34</f>
-        <v>880240.69186146406</v>
+        <f t="shared" si="0"/>
+        <v>3.5209627674458561</v>
       </c>
       <c r="Q34">
-        <f>$T34/G34</f>
-        <v>4960938.1818852546</v>
+        <f t="shared" si="1"/>
+        <v>19.843752727541016</v>
       </c>
       <c r="R34">
-        <f>$T34/J34</f>
-        <v>2007907.7418668496</v>
+        <f t="shared" si="2"/>
+        <v>8.0316309674673985</v>
       </c>
       <c r="S34">
-        <f>$T34/M34</f>
-        <v>4474552.2740033688</v>
+        <f t="shared" si="3"/>
+        <v>17.898209096013474</v>
       </c>
       <c r="T34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1075838976</v>
       </c>
     </row>
@@ -11016,23 +11017,23 @@
         <v>1056</v>
       </c>
       <c r="P35">
-        <f>$T35/D35</f>
-        <v>881906.03079683054</v>
+        <f t="shared" si="0"/>
+        <v>3.527624123187322</v>
       </c>
       <c r="Q35">
-        <f>$T35/G35</f>
-        <v>5103707.6411960134</v>
+        <f t="shared" si="1"/>
+        <v>20.414830564784054</v>
       </c>
       <c r="R35">
-        <f>$T35/J35</f>
-        <v>2010760.7805709415</v>
+        <f t="shared" si="2"/>
+        <v>8.0430431222837662</v>
       </c>
       <c r="S35">
-        <f>$T35/M35</f>
-        <v>4487042.1468178816</v>
+        <f t="shared" si="3"/>
+        <v>17.948168587271521</v>
       </c>
       <c r="T35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1179813888</v>
       </c>
     </row>
@@ -11080,23 +11081,23 @@
         <v>1088</v>
       </c>
       <c r="P36">
-        <f>$T36/D36</f>
-        <v>886218.49801502808</v>
+        <f t="shared" si="0"/>
+        <v>3.5448739920601127</v>
       </c>
       <c r="Q36">
-        <f>$T36/G36</f>
-        <v>5111319.1462390469</v>
+        <f t="shared" si="1"/>
+        <v>20.44527658495619</v>
       </c>
       <c r="R36">
-        <f>$T36/J36</f>
-        <v>2012768.0922489422</v>
+        <f t="shared" si="2"/>
+        <v>8.0510723689957704</v>
       </c>
       <c r="S36">
-        <f>$T36/M36</f>
-        <v>4495501.8535552025</v>
+        <f t="shared" si="3"/>
+        <v>17.98200741422081</v>
       </c>
       <c r="T36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1290280960</v>
       </c>
     </row>
@@ -11144,23 +11145,23 @@
         <v>1120</v>
       </c>
       <c r="P37">
-        <f>$T37/D37</f>
-        <v>874673.29563109821</v>
+        <f t="shared" si="0"/>
+        <v>3.4986931825243928</v>
       </c>
       <c r="Q37">
-        <f>$T37/G37</f>
-        <v>5035245.7990032807</v>
+        <f t="shared" si="1"/>
+        <v>20.140983196013124</v>
       </c>
       <c r="R37">
-        <f>$T37/J37</f>
-        <v>2014246.7666846514</v>
+        <f t="shared" si="2"/>
+        <v>8.056987066738607</v>
       </c>
       <c r="S37">
-        <f>$T37/M37</f>
-        <v>4498859.8114709295</v>
+        <f t="shared" si="3"/>
+        <v>17.995439245883716</v>
       </c>
       <c r="T37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1407436800</v>
       </c>
     </row>
@@ -11208,23 +11209,23 @@
         <v>1152</v>
       </c>
       <c r="P38">
-        <f>$T38/D38</f>
-        <v>884628.67936298903</v>
+        <f t="shared" si="0"/>
+        <v>3.5385147174519558</v>
       </c>
       <c r="Q38">
-        <f>$T38/G38</f>
-        <v>5011102.1834518369</v>
+        <f t="shared" si="1"/>
+        <v>20.044408733807348</v>
       </c>
       <c r="R38">
-        <f>$T38/J38</f>
-        <v>2016522.1781122237</v>
+        <f t="shared" si="2"/>
+        <v>8.0660887124488951</v>
       </c>
       <c r="S38">
-        <f>$T38/M38</f>
-        <v>4510901.1799496925</v>
+        <f t="shared" si="3"/>
+        <v>18.043604719798768</v>
       </c>
       <c r="T38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1531478016</v>
       </c>
     </row>
@@ -11272,23 +11273,23 @@
         <v>1184</v>
       </c>
       <c r="P39">
-        <f>$T39/D39</f>
-        <v>884334.12550663273</v>
+        <f t="shared" si="0"/>
+        <v>3.5373365020265308</v>
       </c>
       <c r="Q39">
-        <f>$T39/G39</f>
-        <v>4919011.2753147231</v>
+        <f t="shared" si="1"/>
+        <v>19.676045101258897</v>
       </c>
       <c r="R39">
-        <f>$T39/J39</f>
-        <v>2018280.8280456585</v>
+        <f t="shared" si="2"/>
+        <v>8.0731233121826342</v>
       </c>
       <c r="S39">
-        <f>$T39/M39</f>
-        <v>4517864.4261234878</v>
+        <f t="shared" si="3"/>
+        <v>18.071457704493948</v>
       </c>
       <c r="T39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1662601216</v>
       </c>
     </row>
@@ -11336,23 +11337,23 @@
         <v>1216</v>
       </c>
       <c r="P40">
-        <f>$T40/D40</f>
-        <v>887093.0919156943</v>
+        <f t="shared" si="0"/>
+        <v>3.5483723676627767</v>
       </c>
       <c r="Q40">
-        <f>$T40/G40</f>
-        <v>4907512.2360615712</v>
+        <f t="shared" si="1"/>
+        <v>19.630048944246283</v>
       </c>
       <c r="R40">
-        <f>$T40/J40</f>
-        <v>2020345.9014867074</v>
+        <f t="shared" si="2"/>
+        <v>8.0813836059468294</v>
       </c>
       <c r="S40">
-        <f>$T40/M40</f>
-        <v>4530300.9161203988</v>
+        <f t="shared" si="3"/>
+        <v>18.121203664481595</v>
       </c>
       <c r="T40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1801003008</v>
       </c>
     </row>
@@ -11400,23 +11401,23 @@
         <v>1248</v>
       </c>
       <c r="P41">
-        <f>$T41/D41</f>
-        <v>882046.72825215315</v>
+        <f t="shared" si="0"/>
+        <v>3.5281869130086125</v>
       </c>
       <c r="Q41">
-        <f>$T41/G41</f>
-        <v>4847036.3288718928</v>
+        <f t="shared" si="1"/>
+        <v>19.38814531548757</v>
       </c>
       <c r="R41">
-        <f>$T41/J41</f>
-        <v>2021934.1974077767</v>
+        <f t="shared" si="2"/>
+        <v>8.0877367896311068</v>
       </c>
       <c r="S41">
-        <f>$T41/M41</f>
-        <v>4537589.4988066824</v>
+        <f t="shared" si="3"/>
+        <v>18.150357995226731</v>
       </c>
       <c r="T41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1946880000</v>
       </c>
     </row>
@@ -11464,23 +11465,23 @@
         <v>1280</v>
       </c>
       <c r="P42">
-        <f>$T42/D42</f>
-        <v>886417.70447802765</v>
+        <f t="shared" si="0"/>
+        <v>3.5456708179121108</v>
       </c>
       <c r="Q42">
-        <f>$T42/G42</f>
-        <v>4776307.076587229</v>
+        <f t="shared" si="1"/>
+        <v>19.10522830634892</v>
       </c>
       <c r="R42">
-        <f>$T42/J42</f>
-        <v>2021878.8082976369</v>
+        <f t="shared" si="2"/>
+        <v>8.0875152331905493</v>
       </c>
       <c r="S42">
-        <f>$T42/M42</f>
-        <v>4539632.191956982</v>
+        <f t="shared" si="3"/>
+        <v>18.158528767827928</v>
       </c>
       <c r="T42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2100428800</v>
       </c>
     </row>
@@ -11528,23 +11529,23 @@
         <v>1312</v>
       </c>
       <c r="P43">
-        <f>$T43/D43</f>
-        <v>883278.27737294685</v>
+        <f t="shared" si="0"/>
+        <v>3.5331131094917874</v>
       </c>
       <c r="Q43">
-        <f>$T43/G43</f>
-        <v>4082791.3898139875</v>
+        <f t="shared" si="1"/>
+        <v>16.33116555925595</v>
       </c>
       <c r="R43">
-        <f>$T43/J43</f>
-        <v>2024820.5253075038</v>
+        <f t="shared" si="2"/>
+        <v>8.0992821012300151</v>
       </c>
       <c r="S43">
-        <f>$T43/M43</f>
-        <v>4551309.3773014648</v>
+        <f t="shared" si="3"/>
+        <v>18.205237509205862</v>
       </c>
       <c r="T43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2261846016</v>
       </c>
     </row>
@@ -11592,23 +11593,23 @@
         <v>1344</v>
       </c>
       <c r="P44">
-        <f>$T44/D44</f>
-        <v>868412.15827183961</v>
+        <f t="shared" si="0"/>
+        <v>3.4736486330873584</v>
       </c>
       <c r="Q44">
-        <f>$T44/G44</f>
-        <v>4673662.930419689</v>
+        <f t="shared" si="1"/>
+        <v>18.694651721678756</v>
       </c>
       <c r="R44">
-        <f>$T44/J44</f>
-        <v>2024504.1475498562</v>
+        <f t="shared" si="2"/>
+        <v>8.0980165901994265</v>
       </c>
       <c r="S44">
-        <f>$T44/M44</f>
-        <v>4551506.4294686625</v>
+        <f t="shared" si="3"/>
+        <v>18.206025717874653</v>
       </c>
       <c r="T44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2431328256</v>
       </c>
     </row>
@@ -11656,23 +11657,23 @@
         <v>1376</v>
       </c>
       <c r="P45">
-        <f>$T45/D45</f>
-        <v>876471.67855307227</v>
+        <f t="shared" si="0"/>
+        <v>3.5058867142122891</v>
       </c>
       <c r="Q45">
-        <f>$T45/G45</f>
-        <v>4661254.8201294895</v>
+        <f t="shared" si="1"/>
+        <v>18.64501928051796</v>
       </c>
       <c r="R45">
-        <f>$T45/J45</f>
-        <v>2026432.3101777059</v>
+        <f t="shared" si="2"/>
+        <v>8.1057292407108239</v>
       </c>
       <c r="S45">
-        <f>$T45/M45</f>
-        <v>4561394.6537526883</v>
+        <f t="shared" si="3"/>
+        <v>18.245578615010754</v>
       </c>
       <c r="T45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2609072128</v>
       </c>
     </row>
@@ -11720,23 +11721,23 @@
         <v>1408</v>
       </c>
       <c r="P46">
-        <f>$T46/D46</f>
-        <v>877683.97057299758</v>
+        <f t="shared" si="0"/>
+        <v>3.510735882291991</v>
       </c>
       <c r="Q46">
-        <f>$T46/G46</f>
-        <v>4579849.0682273209</v>
+        <f t="shared" si="1"/>
+        <v>18.319396272909287</v>
       </c>
       <c r="R46">
-        <f>$T46/J46</f>
-        <v>2028206.5302568567</v>
+        <f t="shared" si="2"/>
+        <v>8.1128261210274264</v>
       </c>
       <c r="S46">
-        <f>$T46/M46</f>
-        <v>4570241.961986511</v>
+        <f t="shared" si="3"/>
+        <v>18.280967847946044</v>
       </c>
       <c r="T46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2795274240</v>
       </c>
     </row>
@@ -11784,23 +11785,23 @@
         <v>1440</v>
       </c>
       <c r="P47">
-        <f>$T47/D47</f>
-        <v>867250.18344871979</v>
+        <f t="shared" si="0"/>
+        <v>3.4690007337948794</v>
       </c>
       <c r="Q47">
-        <f>$T47/G47</f>
-        <v>4356429.4580781274</v>
+        <f t="shared" si="1"/>
+        <v>17.425717832312507</v>
       </c>
       <c r="R47">
-        <f>$T47/J47</f>
-        <v>2028404.0077876442</v>
+        <f t="shared" si="2"/>
+        <v>8.1136160311505758</v>
       </c>
       <c r="S47">
-        <f>$T47/M47</f>
-        <v>4570053.5543980636</v>
+        <f t="shared" si="3"/>
+        <v>18.280214217592256</v>
       </c>
       <c r="T47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2990131200</v>
       </c>
     </row>
@@ -11848,23 +11849,23 @@
         <v>1472</v>
       </c>
       <c r="P48">
-        <f>$T48/D48</f>
-        <v>881382.58064338088</v>
+        <f t="shared" si="0"/>
+        <v>3.5255303225735237</v>
       </c>
       <c r="Q48">
-        <f>$T48/G48</f>
-        <v>4509187.7068344308</v>
+        <f t="shared" si="1"/>
+        <v>18.036750827337723</v>
       </c>
       <c r="R48">
-        <f>$T48/J48</f>
-        <v>2029922.5972110995</v>
+        <f t="shared" si="2"/>
+        <v>8.1196903888443988</v>
       </c>
       <c r="S48">
-        <f>$T48/M48</f>
-        <v>4578620.4901405629</v>
+        <f t="shared" si="3"/>
+        <v>18.314481960562251</v>
       </c>
       <c r="T48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3193839616</v>
       </c>
     </row>
@@ -11912,23 +11913,23 @@
         <v>1504</v>
       </c>
       <c r="P49">
-        <f>$T49/D49</f>
-        <v>882494.40986065462</v>
+        <f t="shared" si="0"/>
+        <v>3.5299776394426186</v>
       </c>
       <c r="Q49">
-        <f>$T49/G49</f>
-        <v>4465201.6342452234</v>
+        <f t="shared" si="1"/>
+        <v>17.860806536980895</v>
       </c>
       <c r="R49">
-        <f>$T49/J49</f>
-        <v>2030201.0155188444</v>
+        <f t="shared" si="2"/>
+        <v>8.1208040620753756</v>
       </c>
       <c r="S49">
-        <f>$T49/M49</f>
-        <v>4579349.0773002971</v>
+        <f t="shared" si="3"/>
+        <v>18.317396309201186</v>
       </c>
       <c r="T49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3406596096</v>
       </c>
     </row>
@@ -11976,23 +11977,23 @@
         <v>1536</v>
       </c>
       <c r="P50">
-        <f>$T50/D50</f>
-        <v>881135.97517295659</v>
+        <f t="shared" si="0"/>
+        <v>3.524543900691826</v>
       </c>
       <c r="Q50">
-        <f>$T50/G50</f>
-        <v>4405695.9234593837</v>
+        <f t="shared" si="1"/>
+        <v>17.622783693837533</v>
       </c>
       <c r="R50">
-        <f>$T50/J50</f>
-        <v>2030859.3061066866</v>
+        <f t="shared" si="2"/>
+        <v>8.1234372244267465</v>
       </c>
       <c r="S50">
-        <f>$T50/M50</f>
-        <v>4586896.186095194</v>
+        <f t="shared" si="3"/>
+        <v>18.347584744380775</v>
       </c>
       <c r="T50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3628597248</v>
       </c>
     </row>
@@ -12040,23 +12041,23 @@
         <v>1568</v>
       </c>
       <c r="P51">
-        <f>$T51/D51</f>
-        <v>880252.59797270317</v>
+        <f t="shared" si="0"/>
+        <v>3.5210103918908127</v>
       </c>
       <c r="Q51">
-        <f>$T51/G51</f>
-        <v>4387301.1442100154</v>
+        <f t="shared" si="1"/>
+        <v>17.549204576840062</v>
       </c>
       <c r="R51">
-        <f>$T51/J51</f>
-        <v>2032113.2075471699</v>
+        <f t="shared" si="2"/>
+        <v>8.1284528301886798</v>
       </c>
       <c r="S51">
-        <f>$T51/M51</f>
-        <v>4589133.7088616928</v>
+        <f t="shared" si="3"/>
+        <v>18.356534835446773</v>
       </c>
       <c r="T51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3860039680</v>
       </c>
     </row>
@@ -12073,7 +12074,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K67"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12103,10 +12104,10 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -12132,10 +12133,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
@@ -12164,12 +12165,12 @@
         <v>32</v>
       </c>
       <c r="I3">
-        <f>K3/D3</f>
-        <v>3630088.7816118319</v>
+        <f>K3*4/(D3/1000)/10^9</f>
+        <v>14.520355126447329</v>
       </c>
       <c r="J3">
-        <f>K3/F3</f>
-        <v>143952.83163191474</v>
+        <f>K3*4/(F3/1000)/10^9</f>
+        <v>0.57581132652765898</v>
       </c>
       <c r="K3">
         <f>H3^3+2*H3^2</f>
@@ -12199,12 +12200,12 @@
         <v>64</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I67" si="0">K4/D4</f>
-        <v>4225769.5409952914</v>
+        <f t="shared" ref="I4:I67" si="0">K4*4/(D4/1000)/10^9</f>
+        <v>16.903078163981164</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J67" si="1">K4/F4</f>
-        <v>647471.05569473514</v>
+        <f t="shared" ref="J4:J67" si="1">K4*4/(F4/1000)/10^9</f>
+        <v>2.5898842227789407</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K67" si="2">H4^3+2*H4^2</f>
@@ -12235,11 +12236,11 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>4617328.8889797758</v>
+        <v>18.469315555919103</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>1251842.416396501</v>
+        <v>5.0073696655860038</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
@@ -12270,11 +12271,11 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>4757694.6874881331</v>
+        <v>19.030778749952535</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>1923751.5467362737</v>
+        <v>7.6950061869450943</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
@@ -12305,11 +12306,11 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>4886515.0706430869</v>
+        <v>19.546060282572348</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>2444187.7460571914</v>
+        <v>9.7767509842287659</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
@@ -12340,11 +12341,11 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>4947400.6073896773</v>
+        <v>19.789602429558709</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>2782415.9919697777</v>
+        <v>11.129663967879113</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
@@ -12375,11 +12376,11 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>5049977.9560099933</v>
+        <v>20.199911824039976</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>3033144.8502388583</v>
+        <v>12.132579400955432</v>
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
@@ -12410,11 +12411,11 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>4984842.8922681417</v>
+        <v>19.939371569072566</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>3288481.7578724418</v>
+        <v>13.153927031489768</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
@@ -12445,11 +12446,11 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>5131249.8666723548</v>
+        <v>20.524999466689419</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>3458554.1621254776</v>
+        <v>13.834216648501911</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
@@ -12480,11 +12481,11 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>5118426.3223418882</v>
+        <v>20.473705289367555</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>3601533.9899357851</v>
+        <v>14.406135959743139</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
@@ -12515,11 +12516,11 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>5180294.0561633334</v>
+        <v>20.721176224653334</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>3731095.7995202364</v>
+        <v>14.924383198080948</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
@@ -12550,11 +12551,11 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>5185679.3002915457</v>
+        <v>20.74271720116618</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>3827656.3865987007</v>
+        <v>15.310625546394801</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
@@ -12585,11 +12586,11 @@
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>5197362.2836450385</v>
+        <v>20.789449134580149</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>3912858.587880197</v>
+        <v>15.651434351520788</v>
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
@@ -12620,11 +12621,11 @@
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>5219688.9574700492</v>
+        <v>20.878755829880195</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>3997928.3693876737</v>
+        <v>15.991713477550695</v>
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
@@ -12655,11 +12656,11 @@
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>5196643.9090130599</v>
+        <v>20.786575636052241</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>4050331.5316103902</v>
+        <v>16.201326126441561</v>
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
@@ -12690,11 +12691,11 @@
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>5195493.8614350054</v>
+        <v>20.78197544574002</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>4111723.9443152617</v>
+        <v>16.446895777261048</v>
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
@@ -12725,11 +12726,11 @@
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>5249154.7415235378</v>
+        <v>20.996618966094154</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>4161221.3174281875</v>
+        <v>16.644885269712752</v>
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
@@ -12760,11 +12761,11 @@
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>5262427.1213231357</v>
+        <v>21.049708485292545</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>4203958.9001155309</v>
+        <v>16.815835600462123</v>
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
@@ -12795,11 +12796,11 @@
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>5260598.7649568766</v>
+        <v>21.042395059827506</v>
       </c>
       <c r="J21">
         <f t="shared" si="1"/>
-        <v>4235197.424642818</v>
+        <v>16.940789698571269</v>
       </c>
       <c r="K21">
         <f t="shared" si="2"/>
@@ -12830,11 +12831,11 @@
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>5317662.5703475568</v>
+        <v>21.270650281390228</v>
       </c>
       <c r="J22">
         <f t="shared" si="1"/>
-        <v>4264079.1056828834</v>
+        <v>17.05631642273153</v>
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
@@ -12865,11 +12866,11 @@
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>5209214.2388928728</v>
+        <v>20.836856955571491</v>
       </c>
       <c r="J23">
         <f t="shared" si="1"/>
-        <v>4290844.4163746117</v>
+        <v>17.163377665498448</v>
       </c>
       <c r="K23">
         <f t="shared" si="2"/>
@@ -12900,11 +12901,11 @@
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>5296341.1407484105</v>
+        <v>21.185364562993641</v>
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
-        <v>4326179.9586552065</v>
+        <v>17.304719834620826</v>
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
@@ -12935,11 +12936,11 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>5304079.4155811416</v>
+        <v>21.21631766232457</v>
       </c>
       <c r="J25">
         <f t="shared" si="1"/>
-        <v>4344182.4034008291</v>
+        <v>17.376729613603317</v>
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
@@ -12970,11 +12971,11 @@
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>5293785.9007832902</v>
+        <v>21.175143603133158</v>
       </c>
       <c r="J26">
         <f t="shared" si="1"/>
-        <v>4365874.6851748601</v>
+        <v>17.463498740699439</v>
       </c>
       <c r="K26">
         <f t="shared" si="2"/>
@@ -13005,11 +13006,11 @@
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>5288351.5731733199</v>
+        <v>21.153406292693283</v>
       </c>
       <c r="J27">
         <f t="shared" si="1"/>
-        <v>4375527.4621292846</v>
+        <v>17.502109848517136</v>
       </c>
       <c r="K27">
         <f t="shared" si="2"/>
@@ -13040,11 +13041,11 @@
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>5273774.4566955036</v>
+        <v>21.095097826782013</v>
       </c>
       <c r="J28">
         <f t="shared" si="1"/>
-        <v>4397717.9073097901</v>
+        <v>17.59087162923916</v>
       </c>
       <c r="K28">
         <f t="shared" si="2"/>
@@ -13075,11 +13076,11 @@
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>5253767.1152720889</v>
+        <v>21.015068461088354</v>
       </c>
       <c r="J29">
         <f t="shared" si="1"/>
-        <v>4418464.4658601601</v>
+        <v>17.673857863440638</v>
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
@@ -13110,11 +13111,11 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>5240031.4578321129</v>
+        <v>20.960125831328455</v>
       </c>
       <c r="J30">
         <f t="shared" si="1"/>
-        <v>4435802.2950315336</v>
+        <v>17.743209180126133</v>
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
@@ -13145,11 +13146,11 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>5226995.2487860909</v>
+        <v>20.907980995144364</v>
       </c>
       <c r="J31">
         <f t="shared" si="1"/>
-        <v>4447745.6974826315</v>
+        <v>17.790982789930531</v>
       </c>
       <c r="K31">
         <f t="shared" si="2"/>
@@ -13180,11 +13181,11 @@
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>5202532.670629588</v>
+        <v>20.810130682518352</v>
       </c>
       <c r="J32">
         <f t="shared" si="1"/>
-        <v>4449046.0371147264</v>
+        <v>17.796184148458906</v>
       </c>
       <c r="K32">
         <f t="shared" si="2"/>
@@ -13215,11 +13216,11 @@
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
-        <v>5153524.7729236474</v>
+        <v>20.614099091694591</v>
       </c>
       <c r="J33">
         <f t="shared" si="1"/>
-        <v>4469502.7507173801</v>
+        <v>17.878011002869517</v>
       </c>
       <c r="K33">
         <f t="shared" si="2"/>
@@ -13250,11 +13251,11 @@
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>4917064.5666988119</v>
+        <v>19.668258266795249</v>
       </c>
       <c r="J34">
         <f t="shared" si="1"/>
-        <v>4475222.3428550037</v>
+        <v>17.900889371420014</v>
       </c>
       <c r="K34">
         <f t="shared" si="2"/>
@@ -13285,11 +13286,11 @@
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>5100067.3833823968</v>
+        <v>20.400269533529588</v>
       </c>
       <c r="J35">
         <f t="shared" si="1"/>
-        <v>4488715.1422918886</v>
+        <v>17.954860569167558</v>
       </c>
       <c r="K35">
         <f t="shared" si="2"/>
@@ -13320,11 +13321,11 @@
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>5070583.5010060361</v>
+        <v>20.282334004024143</v>
       </c>
       <c r="J36">
         <f t="shared" si="1"/>
-        <v>4495501.8535552025</v>
+        <v>17.98200741422081</v>
       </c>
       <c r="K36">
         <f t="shared" si="2"/>
@@ -13355,11 +13356,11 @@
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
-        <v>5020947.2981987996</v>
+        <v>20.083789192795198</v>
       </c>
       <c r="J37">
         <f t="shared" si="1"/>
-        <v>4499837.9026456717</v>
+        <v>17.999351610582686</v>
       </c>
       <c r="K37">
         <f t="shared" si="2"/>
@@ -13390,11 +13391,11 @@
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>4977065.897103413</v>
+        <v>19.908263588413654</v>
       </c>
       <c r="J38">
         <f t="shared" si="1"/>
-        <v>4512655.701379599</v>
+        <v>18.050622805518394</v>
       </c>
       <c r="K38">
         <f t="shared" si="2"/>
@@ -13425,11 +13426,11 @@
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>4786474.9391111089</v>
+        <v>19.145899756444436</v>
       </c>
       <c r="J39">
         <f t="shared" si="1"/>
-        <v>4519190.6887235045</v>
+        <v>18.07676275489402</v>
       </c>
       <c r="K39">
         <f t="shared" si="2"/>
@@ -13460,11 +13461,11 @@
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>4763940.6743570277</v>
+        <v>19.055762697428108</v>
       </c>
       <c r="J40">
         <f t="shared" si="1"/>
-        <v>4530551.634618287</v>
+        <v>18.122206538473147</v>
       </c>
       <c r="K40">
         <f t="shared" si="2"/>
@@ -13495,11 +13496,11 @@
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>4707691.6380729917</v>
+        <v>18.830766552291966</v>
       </c>
       <c r="J41">
         <f t="shared" si="1"/>
-        <v>4538414.5573898889</v>
+        <v>18.153658229559554</v>
       </c>
       <c r="K41">
         <f t="shared" si="2"/>
@@ -13530,11 +13531,11 @@
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>4738667.984198641</v>
+        <v>18.954671936794565</v>
       </c>
       <c r="J42">
         <f t="shared" si="1"/>
-        <v>4541222.2042051787</v>
+        <v>18.164888816820714</v>
       </c>
       <c r="K42">
         <f t="shared" si="2"/>
@@ -13565,11 +13566,11 @@
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
-        <v>4734113.927865779</v>
+        <v>18.936455711463111</v>
       </c>
       <c r="J43">
         <f t="shared" si="1"/>
-        <v>4552087.9566737311</v>
+        <v>18.208351826694923</v>
       </c>
       <c r="K43">
         <f t="shared" si="2"/>
@@ -13600,11 +13601,11 @@
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
-        <v>4661163.7264337223</v>
+        <v>18.644654905734889</v>
       </c>
       <c r="J44">
         <f t="shared" si="1"/>
-        <v>4553253.8091599625</v>
+        <v>18.213015236639851</v>
       </c>
       <c r="K44">
         <f t="shared" si="2"/>
@@ -13635,11 +13636,11 @@
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>4650802.197527959</v>
+        <v>18.603208790111839</v>
       </c>
       <c r="J45">
         <f t="shared" si="1"/>
-        <v>4561099.6124308817</v>
+        <v>18.244398449723526</v>
       </c>
       <c r="K45">
         <f t="shared" si="2"/>
@@ -13670,11 +13671,11 @@
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
-        <v>4651386.9424499338</v>
+        <v>18.605547769799735</v>
       </c>
       <c r="J46">
         <f t="shared" si="1"/>
-        <v>4571168.7143602381</v>
+        <v>18.284674857440951</v>
       </c>
       <c r="K46">
         <f t="shared" si="2"/>
@@ -13705,11 +13706,11 @@
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
-        <v>4577490.4512227802</v>
+        <v>18.309961804891117</v>
       </c>
       <c r="J47">
         <f t="shared" si="1"/>
-        <v>4570360.9051057398</v>
+        <v>18.281443620422959</v>
       </c>
       <c r="K47">
         <f t="shared" si="2"/>
@@ -13740,11 +13741,11 @@
       </c>
       <c r="I48">
         <f t="shared" si="0"/>
-        <v>4523832.9242227012</v>
+        <v>18.095331696890803</v>
       </c>
       <c r="J48">
         <f t="shared" si="1"/>
-        <v>4579427.9815093083</v>
+        <v>18.31771192603723</v>
       </c>
       <c r="K48">
         <f t="shared" si="2"/>
@@ -13775,11 +13776,11 @@
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>4464212.7350640157</v>
+        <v>17.856850940256063</v>
       </c>
       <c r="J49">
         <f t="shared" si="1"/>
-        <v>4580149.4755127225</v>
+        <v>18.320597902050892</v>
       </c>
       <c r="K49">
         <f t="shared" si="2"/>
@@ -13810,11 +13811,11 @@
       </c>
       <c r="I50">
         <f t="shared" si="0"/>
-        <v>4378926.2631991794</v>
+        <v>17.515705052796719</v>
       </c>
       <c r="J50">
         <f t="shared" si="1"/>
-        <v>4587986.52153078</v>
+        <v>18.351946086123121</v>
       </c>
       <c r="K50">
         <f t="shared" si="2"/>
@@ -13845,11 +13846,11 @@
       </c>
       <c r="I51">
         <f t="shared" si="0"/>
-        <v>4331584.6479445379</v>
+        <v>17.326338591778153</v>
       </c>
       <c r="J51">
         <f t="shared" si="1"/>
-        <v>4589002.7700172383</v>
+        <v>18.356011080068953</v>
       </c>
       <c r="K51">
         <f t="shared" si="2"/>
@@ -13880,11 +13881,11 @@
       </c>
       <c r="I52">
         <f t="shared" si="0"/>
-        <v>4344705.938438558</v>
+        <v>17.378823753754229</v>
       </c>
       <c r="J52">
         <f t="shared" si="1"/>
-        <v>4590447.9837206723</v>
+        <v>18.361791934882689</v>
       </c>
       <c r="K52">
         <f t="shared" si="2"/>
@@ -13915,11 +13916,11 @@
       </c>
       <c r="I53">
         <f t="shared" si="0"/>
-        <v>4344865.7874507066</v>
+        <v>17.379463149802827</v>
       </c>
       <c r="J53">
         <f t="shared" si="1"/>
-        <v>4597684.5012154393</v>
+        <v>18.39073800486176</v>
       </c>
       <c r="K53">
         <f t="shared" si="2"/>
@@ -13950,11 +13951,11 @@
       </c>
       <c r="I54">
         <f t="shared" si="0"/>
-        <v>4283772.7965826243</v>
+        <v>17.135091186330499</v>
       </c>
       <c r="J54">
         <f t="shared" si="1"/>
-        <v>4604508.440469536</v>
+        <v>18.418033761878142</v>
       </c>
       <c r="K54">
         <f t="shared" si="2"/>
@@ -13985,11 +13986,11 @@
       </c>
       <c r="I55">
         <f t="shared" si="0"/>
-        <v>4268955.2298293002</v>
+        <v>17.075820919317199</v>
       </c>
       <c r="J55">
         <f t="shared" si="1"/>
-        <v>4606345.6611745628</v>
+        <v>18.425382644698249</v>
       </c>
       <c r="K55">
         <f t="shared" si="2"/>
@@ -14020,11 +14021,11 @@
       </c>
       <c r="I56">
         <f t="shared" si="0"/>
-        <v>4269922.5657133413</v>
+        <v>17.079690262853365</v>
       </c>
       <c r="J56">
         <f t="shared" si="1"/>
-        <v>4610179.5789417317</v>
+        <v>18.440718315766929</v>
       </c>
       <c r="K56">
         <f t="shared" si="2"/>
@@ -14055,11 +14056,11 @@
       </c>
       <c r="I57">
         <f t="shared" si="0"/>
-        <v>4198697.7660163697</v>
+        <v>16.794791064065482</v>
       </c>
       <c r="J57">
         <f t="shared" si="1"/>
-        <v>4609889.7776126079</v>
+        <v>18.439559110450435</v>
       </c>
       <c r="K57">
         <f t="shared" si="2"/>
@@ -14090,11 +14091,11 @@
       </c>
       <c r="I58">
         <f t="shared" si="0"/>
-        <v>4199229.9959181296</v>
+        <v>16.796919983672517</v>
       </c>
       <c r="J58">
         <f t="shared" si="1"/>
-        <v>4619004.8555209907</v>
+        <v>18.476019422083962</v>
       </c>
       <c r="K58">
         <f t="shared" si="2"/>
@@ -14125,11 +14126,11 @@
       </c>
       <c r="I59">
         <f t="shared" si="0"/>
-        <v>4203581.6082091872</v>
+        <v>16.814326432836751</v>
       </c>
       <c r="J59">
         <f t="shared" si="1"/>
-        <v>4619218.9420379112</v>
+        <v>18.476875768151643</v>
       </c>
       <c r="K59">
         <f t="shared" si="2"/>
@@ -14160,11 +14161,11 @@
       </c>
       <c r="I60">
         <f t="shared" si="0"/>
-        <v>4145230.9477856504</v>
+        <v>16.580923791142602</v>
       </c>
       <c r="J60">
         <f t="shared" si="1"/>
-        <v>4623773.3077112017</v>
+        <v>18.495093230844805</v>
       </c>
       <c r="K60">
         <f t="shared" si="2"/>
@@ -14195,11 +14196,11 @@
       </c>
       <c r="I61">
         <f t="shared" si="0"/>
-        <v>4077586.3454787559</v>
+        <v>16.310345381915024</v>
       </c>
       <c r="J61">
         <f t="shared" si="1"/>
-        <v>4624955.8304614667</v>
+        <v>18.499823321845867</v>
       </c>
       <c r="K61">
         <f t="shared" si="2"/>
@@ -14230,11 +14231,11 @@
       </c>
       <c r="I62">
         <f t="shared" si="0"/>
-        <v>4154262.4623286468</v>
+        <v>16.617049849314586</v>
       </c>
       <c r="J62">
         <f t="shared" si="1"/>
-        <v>4624028.9244062733</v>
+        <v>18.49611569762509</v>
       </c>
       <c r="K62">
         <f t="shared" si="2"/>
@@ -14265,11 +14266,11 @@
       </c>
       <c r="I63">
         <f t="shared" si="0"/>
-        <v>4111763.1553950319</v>
+        <v>16.447052621580127</v>
       </c>
       <c r="J63">
         <f t="shared" si="1"/>
-        <v>4630960.4324109145</v>
+        <v>18.523841729643657</v>
       </c>
       <c r="K63">
         <f t="shared" si="2"/>
@@ -14300,11 +14301,11 @@
       </c>
       <c r="I64">
         <f t="shared" si="0"/>
-        <v>4104874.1433087238</v>
+        <v>16.419496573234895</v>
       </c>
       <c r="J64">
         <f t="shared" si="1"/>
-        <v>4633908.9602845283</v>
+        <v>18.535635841138117</v>
       </c>
       <c r="K64">
         <f t="shared" si="2"/>
@@ -14335,11 +14336,11 @@
       </c>
       <c r="I65">
         <f t="shared" si="0"/>
-        <v>4114515.0665964335</v>
+        <v>16.458060266385733</v>
       </c>
       <c r="J65">
         <f t="shared" si="1"/>
-        <v>4628872.9903772892</v>
+        <v>18.515491961509159</v>
       </c>
       <c r="K65">
         <f t="shared" si="2"/>
@@ -14370,11 +14371,11 @@
       </c>
       <c r="I66">
         <f t="shared" si="0"/>
-        <v>4027959.1129266489</v>
+        <v>16.111836451706598</v>
       </c>
       <c r="J66">
         <f t="shared" si="1"/>
-        <v>4643299.7618494742</v>
+        <v>18.573199047397896</v>
       </c>
       <c r="K66">
         <f t="shared" si="2"/>
@@ -14405,11 +14406,11 @@
       </c>
       <c r="I67">
         <f t="shared" si="0"/>
-        <v>4080455.5400024466</v>
+        <v>16.321822160009784</v>
       </c>
       <c r="J67">
         <f t="shared" si="1"/>
-        <v>4633401.8157969192</v>
+        <v>18.533607263187676</v>
       </c>
       <c r="K67">
         <f t="shared" si="2"/>

</xml_diff>